<commit_message>
made type split a little more complex
</commit_message>
<xml_diff>
--- a/Data/model_outputs_baseline/UFA/i_AB_UFA.xlsx
+++ b/Data/model_outputs_baseline/UFA/i_AB_UFA.xlsx
@@ -450,7 +450,7 @@
         <v>1600</v>
       </c>
       <c r="B2" t="n">
-        <v>1523802.704100378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -458,7 +458,7 @@
         <v>1601</v>
       </c>
       <c r="B3" t="n">
-        <v>1835.268315311871</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -466,7 +466,7 @@
         <v>1602</v>
       </c>
       <c r="B4" t="n">
-        <v>1864.5399992335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -474,7 +474,7 @@
         <v>1603</v>
       </c>
       <c r="B5" t="n">
-        <v>1894.450506100898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -482,7 +482,7 @@
         <v>1604</v>
       </c>
       <c r="B6" t="n">
-        <v>1925.021848104422</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -490,7 +490,7 @@
         <v>1605</v>
       </c>
       <c r="B7" t="n">
-        <v>1956.276927885651</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -498,7 +498,7 @@
         <v>1606</v>
       </c>
       <c r="B8" t="n">
-        <v>1988.239564685683</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -506,7 +506,7 @@
         <v>1607</v>
       </c>
       <c r="B9" t="n">
-        <v>2020.934520250054</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -514,7 +514,7 @@
         <v>1608</v>
       </c>
       <c r="B10" t="n">
-        <v>2054.387524398654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -522,7 +522,7 @@
         <v>1609</v>
       </c>
       <c r="B11" t="n">
-        <v>2088.625300136805</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -530,7 +530,7 @@
         <v>1610</v>
       </c>
       <c r="B12" t="n">
-        <v>2123.675588224809</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -538,7 +538,7 @@
         <v>1611</v>
       </c>
       <c r="B13" t="n">
-        <v>2159.567171095516</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -546,7 +546,7 @@
         <v>1612</v>
       </c>
       <c r="B14" t="n">
-        <v>2196.329895975816</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -554,7 +554,7 @@
         <v>1613</v>
       </c>
       <c r="B15" t="n">
-        <v>2233.994697128299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -562,7 +562,7 @@
         <v>1614</v>
       </c>
       <c r="B16" t="n">
-        <v>2272.593617046733</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -570,7 +570,7 @@
         <v>1615</v>
       </c>
       <c r="B17" t="n">
-        <v>2312.159826507774</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -578,7 +578,7 @@
         <v>1616</v>
       </c>
       <c r="B18" t="n">
-        <v>2352.727643309576</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -586,7 +586,7 @@
         <v>1617</v>
       </c>
       <c r="B19" t="n">
-        <v>2394.332549574562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -594,7 +594,7 @@
         <v>1618</v>
       </c>
       <c r="B20" t="n">
-        <v>2437.011207464494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -602,7 +602,7 @@
         <v>1619</v>
       </c>
       <c r="B21" t="n">
-        <v>2480.801473141095</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -610,7 +610,7 @@
         <v>1620</v>
       </c>
       <c r="B22" t="n">
-        <v>2525.74240884419</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -618,7 +618,7 @@
         <v>1621</v>
       </c>
       <c r="B23" t="n">
-        <v>2571.874292896148</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -626,7 +626,7 @@
         <v>1622</v>
       </c>
       <c r="B24" t="n">
-        <v>2619.238627488875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -634,7 +634,7 @@
         <v>1623</v>
       </c>
       <c r="B25" t="n">
-        <v>2667.878144088119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -642,7 +642,7 @@
         <v>1624</v>
       </c>
       <c r="B26" t="n">
-        <v>2717.83680626683</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -650,7 +650,7 @@
         <v>1625</v>
       </c>
       <c r="B27" t="n">
-        <v>2769.159809824145</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -658,7 +658,7 @@
         <v>1626</v>
       </c>
       <c r="B28" t="n">
-        <v>2821.893579995086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -666,7 +666,7 @@
         <v>1627</v>
       </c>
       <c r="B29" t="n">
-        <v>2876.085765589462</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -674,7 +674,7 @@
         <v>1628</v>
       </c>
       <c r="B30" t="n">
-        <v>2931.785229892854</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -682,7 +682,7 @@
         <v>1629</v>
       </c>
       <c r="B31" t="n">
-        <v>2989.042038139976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -690,7 +690,7 @@
         <v>1630</v>
       </c>
       <c r="B32" t="n">
-        <v>3047.907441408186</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -698,7 +698,7 @@
         <v>1631</v>
       </c>
       <c r="B33" t="n">
-        <v>3108.433856755109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -706,7 +706,7 @@
         <v>1632</v>
       </c>
       <c r="B34" t="n">
-        <v>3170.674843432228</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -714,7 +714,7 @@
         <v>1633</v>
       </c>
       <c r="B35" t="n">
-        <v>3234.68507502193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -722,7 +722,7 @@
         <v>1634</v>
       </c>
       <c r="B36" t="n">
-        <v>3300.520307330631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -730,7 +730,7 @@
         <v>1635</v>
       </c>
       <c r="B37" t="n">
-        <v>3368.237341900593</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -738,7 +738,7 @@
         <v>1636</v>
       </c>
       <c r="B38" t="n">
-        <v>3437.893984976781</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -746,7 +746,7 @@
         <v>1637</v>
       </c>
       <c r="B39" t="n">
-        <v>3509.549001816239</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -754,7 +754,7 @@
         <v>1638</v>
       </c>
       <c r="B40" t="n">
-        <v>3583.262066193772</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41">
@@ -762,7 +762,7 @@
         <v>1639</v>
       </c>
       <c r="B41" t="n">
-        <v>3659.093704993789</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -770,7 +770,7 @@
         <v>1640</v>
       </c>
       <c r="B42" t="n">
-        <v>3737.105237769291</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -778,7 +778,7 @@
         <v>1641</v>
       </c>
       <c r="B43" t="n">
-        <v>3817.358711202191</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -786,7 +786,7 @@
         <v>1642</v>
       </c>
       <c r="B44" t="n">
-        <v>3899.916828336336</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -794,7 +794,7 @@
         <v>1643</v>
       </c>
       <c r="B45" t="n">
-        <v>3984.842872558369</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -802,7 +802,7 @@
         <v>1644</v>
       </c>
       <c r="B46" t="n">
-        <v>4072.200626242578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47">
@@ -810,7 +810,7 @@
         <v>1645</v>
       </c>
       <c r="B47" t="n">
-        <v>4162.054284026524</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48">
@@ -818,7 +818,7 @@
         <v>1646</v>
       </c>
       <c r="B48" t="n">
-        <v>4254.46836071837</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -826,7 +826,7 @@
         <v>1647</v>
       </c>
       <c r="B49" t="n">
-        <v>4349.507593794252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50">
@@ -834,7 +834,7 @@
         <v>1648</v>
       </c>
       <c r="B50" t="n">
-        <v>4447.236840529513</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -842,7 +842,7 @@
         <v>1649</v>
       </c>
       <c r="B51" t="n">
-        <v>4547.720969796788</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -850,7 +850,7 @@
         <v>1650</v>
       </c>
       <c r="B52" t="n">
-        <v>4651.024748569576</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -858,7 +858,7 @@
         <v>1651</v>
       </c>
       <c r="B53" t="n">
-        <v>4757.212723229521</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -866,7 +866,7 @@
         <v>1652</v>
       </c>
       <c r="B54" t="n">
-        <v>4866.349095757594</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -874,7 +874,7 @@
         <v>1653</v>
       </c>
       <c r="B55" t="n">
-        <v>4978.49759496048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -882,7 +882,7 @@
         <v>1654</v>
       </c>
       <c r="B56" t="n">
-        <v>5093.72134284242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57">
@@ -890,7 +890,7 @@
         <v>1655</v>
       </c>
       <c r="B57" t="n">
-        <v>5212.082716322776</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58">
@@ -898,7 +898,7 @@
         <v>1656</v>
       </c>
       <c r="B58" t="n">
-        <v>5333.643204496357</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59">
@@ -906,7 +906,7 @@
         <v>1657</v>
       </c>
       <c r="B59" t="n">
-        <v>5458.463261629106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -914,7 +914,7 @@
         <v>1658</v>
       </c>
       <c r="B60" t="n">
-        <v>5586.602156169736</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61">
@@ -922,7 +922,7 @@
         <v>1659</v>
       </c>
       <c r="B61" t="n">
-        <v>5718.117816039652</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62">
@@ -930,7 +930,7 @@
         <v>1660</v>
       </c>
       <c r="B62" t="n">
-        <v>5853.066670493892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -938,7 +938,7 @@
         <v>1661</v>
       </c>
       <c r="B63" t="n">
-        <v>5991.503488881307</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64">
@@ -946,7 +946,7 @@
         <v>1662</v>
       </c>
       <c r="B64" t="n">
-        <v>6133.481216678803</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
@@ -954,7 +954,7 @@
         <v>1663</v>
       </c>
       <c r="B65" t="n">
-        <v>6279.050809127719</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66">
@@ -962,7 +962,7 @@
         <v>1664</v>
       </c>
       <c r="B66" t="n">
-        <v>6428.261062942261</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67">
@@ -970,7 +970,7 @@
         <v>1665</v>
       </c>
       <c r="B67" t="n">
-        <v>6581.158446452024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -978,7 +978,7 @@
         <v>1666</v>
       </c>
       <c r="B68" t="n">
-        <v>6737.786928678492</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69">
@@ -986,7 +986,7 @@
         <v>1667</v>
       </c>
       <c r="B69" t="n">
-        <v>6898.187807807837</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
@@ -994,7 +994,7 @@
         <v>1668</v>
       </c>
       <c r="B70" t="n">
-        <v>7062.399539550543</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1002,7 +1002,7 @@
         <v>1669</v>
       </c>
       <c r="B71" t="n">
-        <v>7230.457565913514</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72">
@@ -1010,7 +1010,7 @@
         <v>1670</v>
       </c>
       <c r="B72" t="n">
-        <v>7402.394144943423</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73">
@@ -1018,7 +1018,7 @@
         <v>1671</v>
       </c>
       <c r="B73" t="n">
-        <v>7578.238181969085</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74">
@@ -1026,7 +1026,7 @@
         <v>1672</v>
       </c>
       <c r="B74" t="n">
-        <v>7758.01506295455</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1034,7 +1034,7 @@
         <v>1673</v>
       </c>
       <c r="B75" t="n">
-        <v>7941.746490537299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76">
@@ -1042,7 +1042,7 @@
         <v>1674</v>
       </c>
       <c r="B76" t="n">
-        <v>8129.450323368359</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1050,7 +1050,7 @@
         <v>1675</v>
       </c>
       <c r="B77" t="n">
-        <v>8321.140419373971</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78">
@@ -1058,7 +1058,7 @@
         <v>1676</v>
       </c>
       <c r="B78" t="n">
-        <v>8516.826483578903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79">
@@ -1066,7 +1066,7 @@
         <v>1677</v>
       </c>
       <c r="B79" t="n">
-        <v>8716.513921117235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80">
@@ -1074,7 +1074,7 @@
         <v>1678</v>
       </c>
       <c r="B80" t="n">
-        <v>8920.203696097047</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81">
@@ -1082,7 +1082,7 @@
         <v>1679</v>
       </c>
       <c r="B81" t="n">
-        <v>9127.892196955065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82">
@@ -1090,7 +1090,7 @@
         <v>1680</v>
       </c>
       <c r="B82" t="n">
-        <v>9339.571108961636</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1098,7 +1098,7 @@
         <v>1681</v>
       </c>
       <c r="B83" t="n">
-        <v>9555.227294525668</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84">
@@ -1106,7 +1106,7 @@
         <v>1682</v>
       </c>
       <c r="B84" t="n">
-        <v>9774.842681950066</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85">
@@ -1114,7 +1114,7 @@
         <v>1683</v>
       </c>
       <c r="B85" t="n">
-        <v>9998.394163274123</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86">
@@ -1122,7 +1122,7 @@
         <v>1684</v>
       </c>
       <c r="B86" t="n">
-        <v>10225.85350184494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1130,7 +1130,7 @@
         <v>1685</v>
       </c>
       <c r="B87" t="n">
-        <v>10457.18725021313</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88">
@@ -1138,7 +1138,7 @@
         <v>1686</v>
       </c>
       <c r="B88" t="n">
-        <v>10692.3566789964</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89">
@@ -1146,7 +1146,7 @@
         <v>1687</v>
       </c>
       <c r="B89" t="n">
-        <v>10931.31771727457</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
@@ -1154,7 +1154,7 @@
         <v>1688</v>
       </c>
       <c r="B90" t="n">
-        <v>11174.02090506212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91">
@@ -1162,7 +1162,7 @@
         <v>1689</v>
       </c>
       <c r="B91" t="n">
-        <v>11420.41135845205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92">
@@ -1170,7 +1170,7 @@
         <v>1690</v>
       </c>
       <c r="B92" t="n">
-        <v>11670.42874790532</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93">
@@ -1178,7 +1178,7 @@
         <v>1691</v>
       </c>
       <c r="B93" t="n">
-        <v>11924.00729017681</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -1186,7 +1186,7 @@
         <v>1692</v>
       </c>
       <c r="B94" t="n">
-        <v>12181.07575434983</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -1194,7 +1194,7 @@
         <v>1693</v>
       </c>
       <c r="B95" t="n">
-        <v>12441.55748238496</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96">
@@ -1202,7 +1202,7 @@
         <v>1694</v>
       </c>
       <c r="B96" t="n">
-        <v>12705.37042455201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -1210,7 +1210,7 @@
         <v>1695</v>
       </c>
       <c r="B97" t="n">
-        <v>12972.42719010782</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98">
@@ -1218,7 +1218,7 @@
         <v>1696</v>
       </c>
       <c r="B98" t="n">
-        <v>13242.63511349696</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99">
@@ -1226,7 +1226,7 @@
         <v>1697</v>
       </c>
       <c r="B99" t="n">
-        <v>13515.89633633472</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100">
@@ -1234,7 +1234,7 @@
         <v>1698</v>
       </c>
       <c r="B100" t="n">
-        <v>13792.1079053715</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101">
@@ -1242,7 +1242,7 @@
         <v>1699</v>
       </c>
       <c r="B101" t="n">
-        <v>14071.16188657976</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102">
@@ -1250,7 +1250,7 @@
         <v>1700</v>
       </c>
       <c r="B102" t="n">
-        <v>14352.94549549541</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103">
@@ -1258,7 +1258,7 @@
         <v>1701</v>
       </c>
       <c r="B103" t="n">
-        <v>14637.34124381914</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104">
@@ -1266,7 +1266,7 @@
         <v>1702</v>
       </c>
       <c r="B104" t="n">
-        <v>14924.22710228483</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105">
@@ -1274,7 +1274,7 @@
         <v>1703</v>
       </c>
       <c r="B105" t="n">
-        <v>15213.47667975435</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106">
@@ -1282,7 +1282,7 @@
         <v>1704</v>
       </c>
       <c r="B106" t="n">
-        <v>15504.95941835819</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -1290,7 +1290,7 @@
         <v>1705</v>
       </c>
       <c r="B107" t="n">
-        <v>15798.54080455906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -1298,7 +1298,7 @@
         <v>1706</v>
       </c>
       <c r="B108" t="n">
-        <v>16094.08259584263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109">
@@ -1306,7 +1306,7 @@
         <v>1707</v>
       </c>
       <c r="B109" t="n">
-        <v>16391.44306277197</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110">
@@ -1314,7 +1314,7 @@
         <v>1708</v>
       </c>
       <c r="B110" t="n">
-        <v>16690.47724602214</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111">
@@ -1322,7 +1322,7 @@
         <v>1709</v>
       </c>
       <c r="B111" t="n">
-        <v>16991.03722796838</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112">
@@ -1330,7 +1330,7 @@
         <v>1710</v>
       </c>
       <c r="B112" t="n">
-        <v>17292.97241836205</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113">
@@ -1338,7 +1338,7 @@
         <v>1711</v>
       </c>
       <c r="B113" t="n">
-        <v>17596.12985352441</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -1346,7 +1346,7 @@
         <v>1712</v>
       </c>
       <c r="B114" t="n">
-        <v>17900.35450848839</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115">
@@ -1354,7 +1354,7 @@
         <v>1713</v>
       </c>
       <c r="B115" t="n">
-        <v>18205.4896214024</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -1362,7 +1362,7 @@
         <v>1714</v>
       </c>
       <c r="B116" t="n">
-        <v>18511.37702949534</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -1370,7 +1370,7 @@
         <v>1715</v>
       </c>
       <c r="B117" t="n">
-        <v>18817.85751583263</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -1378,7 +1378,7 @@
         <v>1716</v>
       </c>
       <c r="B118" t="n">
-        <v>19124.77116604725</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -1386,7 +1386,7 @@
         <v>1717</v>
       </c>
       <c r="B119" t="n">
-        <v>19431.95773415994</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -1394,7 +1394,7 @@
         <v>1718</v>
       </c>
       <c r="B120" t="n">
-        <v>19739.25701659247</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121">
@@ -1402,7 +1402,7 @@
         <v>1719</v>
       </c>
       <c r="B121" t="n">
-        <v>20046.50923339774</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -1410,7 +1410,7 @@
         <v>1720</v>
       </c>
       <c r="B122" t="n">
-        <v>20353.55541571225</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123">
@@ -1418,7 +1418,7 @@
         <v>1721</v>
       </c>
       <c r="B123" t="n">
-        <v>20660.23779838289</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124">
@@ -1426,7 +1426,7 @@
         <v>1722</v>
       </c>
       <c r="B124" t="n">
-        <v>20966.40021669956</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125">
@@ -1434,7 +1434,7 @@
         <v>1723</v>
       </c>
       <c r="B125" t="n">
-        <v>21271.88850612436</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -1442,7 +1442,7 @@
         <v>1724</v>
       </c>
       <c r="B126" t="n">
-        <v>21576.55090388823</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127">
@@ -1450,7 +1450,7 @@
         <v>1725</v>
       </c>
       <c r="B127" t="n">
-        <v>21880.23845128947</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -1458,7 +1458,7 @@
         <v>1726</v>
       </c>
       <c r="B128" t="n">
-        <v>22182.80539553936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -1466,7 +1466,7 @@
         <v>1727</v>
       </c>
       <c r="B129" t="n">
-        <v>22484.10958993908</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -1474,7 +1474,7 @@
         <v>1728</v>
       </c>
       <c r="B130" t="n">
-        <v>22784.01289122892</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -1482,7 +1482,7 @@
         <v>1729</v>
       </c>
       <c r="B131" t="n">
-        <v>23082.38155285441</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -1490,7 +1490,7 @@
         <v>1730</v>
       </c>
       <c r="B132" t="n">
-        <v>23379.08661300578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -1498,7 +1498,7 @@
         <v>1731</v>
       </c>
       <c r="B133" t="n">
-        <v>23674.00427619218</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
@@ -1506,7 +1506,7 @@
         <v>1732</v>
       </c>
       <c r="B134" t="n">
-        <v>23967.01628715926</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -1514,7 +1514,7 @@
         <v>1733</v>
       </c>
       <c r="B135" t="n">
-        <v>24258.01029602517</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136">
@@ -1522,7 +1522,7 @@
         <v>1734</v>
       </c>
       <c r="B136" t="n">
-        <v>24546.88021339689</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137">
@@ -1530,7 +1530,7 @@
         <v>1735</v>
       </c>
       <c r="B137" t="n">
-        <v>24833.52655442112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -1538,7 +1538,7 @@
         <v>1736</v>
       </c>
       <c r="B138" t="n">
-        <v>25117.8567706102</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139">
@@ -1546,7 +1546,7 @@
         <v>1737</v>
       </c>
       <c r="B139" t="n">
-        <v>25399.78556837878</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140">
@@ -1554,7 +1554,7 @@
         <v>1738</v>
       </c>
       <c r="B140" t="n">
-        <v>25679.23521328903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141">
@@ -1562,7 +1562,7 @@
         <v>1739</v>
       </c>
       <c r="B141" t="n">
-        <v>25956.13581897818</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142">
@@ -1570,7 +1570,7 @@
         <v>1740</v>
       </c>
       <c r="B142" t="n">
-        <v>26230.42561983431</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -1578,7 +1578,7 @@
         <v>1741</v>
       </c>
       <c r="B143" t="n">
-        <v>26502.05122654753</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144">
@@ -1586,7 +1586,7 @@
         <v>1742</v>
       </c>
       <c r="B144" t="n">
-        <v>26770.96786365323</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -1594,7 +1594,7 @@
         <v>1743</v>
       </c>
       <c r="B145" t="n">
-        <v>27037.13958833317</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -1602,7 +1602,7 @@
         <v>1744</v>
       </c>
       <c r="B146" t="n">
-        <v>27300.53948970293</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -1610,7 +1610,7 @@
         <v>1745</v>
       </c>
       <c r="B147" t="n">
-        <v>27561.14986798655</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -1618,7 +1618,7 @@
         <v>1746</v>
       </c>
       <c r="B148" t="n">
-        <v>27818.96239292214</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -1626,7 +1626,7 @@
         <v>1747</v>
       </c>
       <c r="B149" t="n">
-        <v>28073.9782409385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
@@ -1634,7 +1634,7 @@
         <v>1748</v>
       </c>
       <c r="B150" t="n">
-        <v>28326.20821062838</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -1642,7 +1642,7 @@
         <v>1749</v>
       </c>
       <c r="B151" t="n">
-        <v>28575.67281612564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152">
@@ -1650,7 +1650,7 @@
         <v>1750</v>
       </c>
       <c r="B152" t="n">
-        <v>28822.4023581418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153">
@@ -1658,7 +1658,7 @@
         <v>1751</v>
       </c>
       <c r="B153" t="n">
-        <v>29066.43697238156</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154">
@@ -1666,7 +1666,7 @@
         <v>1752</v>
       </c>
       <c r="B154" t="n">
-        <v>29307.8266552523</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -1674,7 +1674,7 @@
         <v>1753</v>
       </c>
       <c r="B155" t="n">
-        <v>29546.63126675893</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156">
@@ -1682,7 +1682,7 @@
         <v>1754</v>
       </c>
       <c r="B156" t="n">
-        <v>29782.92051062172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -1690,7 +1690,7 @@
         <v>1755</v>
       </c>
       <c r="B157" t="n">
-        <v>30016.77389173805</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -1698,7 +1698,7 @@
         <v>1756</v>
       </c>
       <c r="B158" t="n">
-        <v>30248.28065109842</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
@@ -1706,7 +1706,7 @@
         <v>1757</v>
       </c>
       <c r="B159" t="n">
-        <v>30477.53967849187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
@@ -1714,7 +1714,7 @@
         <v>1758</v>
       </c>
       <c r="B160" t="n">
-        <v>30704.65940326455</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -1722,7 +1722,7 @@
         <v>1759</v>
       </c>
       <c r="B161" t="n">
-        <v>30929.75766358119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -1730,7 +1730,7 @@
         <v>1760</v>
       </c>
       <c r="B162" t="n">
-        <v>31152.96155465303</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -1738,7 +1738,7 @@
         <v>1761</v>
       </c>
       <c r="B163" t="n">
-        <v>31374.40725649122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -1746,7 +1746,7 @@
         <v>1762</v>
       </c>
       <c r="B164" t="n">
-        <v>31594.2398418199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="165">
@@ -1754,7 +1754,7 @@
         <v>1763</v>
       </c>
       <c r="B165" t="n">
-        <v>31812.61306481022</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166">
@@ -1762,7 +1762,7 @@
         <v>1764</v>
       </c>
       <c r="B166" t="n">
-        <v>32029.68913143372</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -1770,7 +1770,7 @@
         <v>1765</v>
       </c>
       <c r="B167" t="n">
-        <v>32245.6384522312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -1778,7 +1778,7 @@
         <v>1766</v>
       </c>
       <c r="B168" t="n">
-        <v>32460.63937836234</v>
+        <v>0</v>
       </c>
     </row>
     <row r="169">
@@ -1786,7 +1786,7 @@
         <v>1767</v>
       </c>
       <c r="B169" t="n">
-        <v>32674.87792188481</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170">
@@ -1794,7 +1794,7 @@
         <v>1768</v>
       </c>
       <c r="B170" t="n">
-        <v>32888.54746124559</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171">
@@ -1802,7 +1802,7 @@
         <v>1769</v>
       </c>
       <c r="B171" t="n">
-        <v>33101.84843299208</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -1810,7 +1810,7 @@
         <v>1770</v>
       </c>
       <c r="B172" t="n">
-        <v>33314.98801079053</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173">
@@ -1818,7 +1818,7 @@
         <v>1771</v>
       </c>
       <c r="B173" t="n">
-        <v>33528.17977285293</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -1826,7 +1826,7 @@
         <v>1772</v>
       </c>
       <c r="B174" t="n">
-        <v>33741.64335891618</v>
+        <v>0</v>
       </c>
     </row>
     <row r="175">
@@ -1834,7 +1834,7 @@
         <v>1773</v>
       </c>
       <c r="B175" t="n">
-        <v>33955.60411793276</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
@@ -1842,7 +1842,7 @@
         <v>1774</v>
       </c>
       <c r="B176" t="n">
-        <v>34170.29274768265</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -1850,7 +1850,7 @@
         <v>1775</v>
       </c>
       <c r="B177" t="n">
-        <v>34385.94492751306</v>
+        <v>0</v>
       </c>
     </row>
     <row r="178">
@@ -1858,7 +1858,7 @@
         <v>1776</v>
       </c>
       <c r="B178" t="n">
-        <v>34602.80094542669</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179">
@@ -1866,7 +1866,7 @@
         <v>1777</v>
       </c>
       <c r="B179" t="n">
-        <v>34821.10532077106</v>
+        <v>0</v>
       </c>
     </row>
     <row r="180">
@@ -1874,7 +1874,7 @@
         <v>1778</v>
       </c>
       <c r="B180" t="n">
-        <v>35041.10642375534</v>
+        <v>0</v>
       </c>
     </row>
     <row r="181">
@@ -1882,7 +1882,7 @@
         <v>1779</v>
       </c>
       <c r="B181" t="n">
-        <v>35263.05609305537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182">
@@ -1890,7 +1890,7 @@
         <v>1780</v>
       </c>
       <c r="B182" t="n">
-        <v>35487.20925273945</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183">
@@ -1898,7 +1898,7 @@
         <v>1781</v>
       </c>
       <c r="B183" t="n">
-        <v>35713.8235297385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184">
@@ -1906,7 +1906,7 @@
         <v>1782</v>
       </c>
       <c r="B184" t="n">
-        <v>35943.15887308119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185">
@@ -1914,7 +1914,7 @@
         <v>1783</v>
       </c>
       <c r="B185" t="n">
-        <v>36175.47717611366</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186">
@@ -1922,7 +1922,7 @@
         <v>1784</v>
       </c>
       <c r="B186" t="n">
-        <v>36411.04190284799</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187">
@@ -1930,7 +1930,7 @@
         <v>1785</v>
       </c>
       <c r="B187" t="n">
-        <v>36650.11771961203</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -1938,7 +1938,7 @@
         <v>1786</v>
       </c>
       <c r="B188" t="n">
-        <v>36892.97013313506</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -1946,7 +1946,7 @@
         <v>1787</v>
       </c>
       <c r="B189" t="n">
-        <v>37139.8651361119</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190">
@@ -1954,7 +1954,7 @@
         <v>1788</v>
       </c>
       <c r="B190" t="n">
-        <v>37391.06886136497</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191">
@@ -1962,7 +1962,7 @@
         <v>1789</v>
       </c>
       <c r="B191" t="n">
-        <v>37646.84724555262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -1970,7 +1970,7 @@
         <v>1790</v>
       </c>
       <c r="B192" t="n">
-        <v>37907.46570341672</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -1978,7 +1978,7 @@
         <v>1791</v>
       </c>
       <c r="B193" t="n">
-        <v>38173.1888135272</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194">
@@ -1986,7 +1986,7 @@
         <v>1792</v>
       </c>
       <c r="B194" t="n">
-        <v>38444.2800163221</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195">
@@ -1994,7 +1994,7 @@
         <v>1793</v>
       </c>
       <c r="B195" t="n">
-        <v>38721.00132532595</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196">
@@ -2002,7 +2002,7 @@
         <v>1794</v>
       </c>
       <c r="B196" t="n">
-        <v>39003.61305230527</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197">
@@ -2010,7 +2010,7 @@
         <v>1795</v>
       </c>
       <c r="B197" t="n">
-        <v>39292.37354705519</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198">
@@ -2018,7 +2018,7 @@
         <v>1796</v>
       </c>
       <c r="B198" t="n">
-        <v>39587.53895249086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199">
@@ -2026,7 +2026,7 @@
         <v>1797</v>
       </c>
       <c r="B199" t="n">
-        <v>39889.36297565229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200">
@@ -2034,7 +2034,7 @@
         <v>1798</v>
       </c>
       <c r="B200" t="n">
-        <v>40198.09667513843</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201">
@@ -2042,7 +2042,7 @@
         <v>1799</v>
       </c>
       <c r="B201" t="n">
-        <v>40513.98826548934</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202">
@@ -2050,7 +2050,7 @@
         <v>1800</v>
       </c>
       <c r="B202" t="n">
-        <v>40837.28293891459</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203">
@@ -2058,7 +2058,7 @@
         <v>1801</v>
       </c>
       <c r="B203" t="n">
-        <v>41168.2318912167</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204">
@@ -2066,7 +2066,7 @@
         <v>1802</v>
       </c>
       <c r="B204" t="n">
-        <v>41507.05644771336</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205">
@@ -2074,7 +2074,7 @@
         <v>1803</v>
       </c>
       <c r="B205" t="n">
-        <v>41854.00009261468</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206">
@@ -2082,7 +2082,7 @@
         <v>1804</v>
       </c>
       <c r="B206" t="n">
-        <v>42209.29450933033</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207">
@@ -2090,7 +2090,7 @@
         <v>1805</v>
       </c>
       <c r="B207" t="n">
-        <v>42573.16773875563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208">
@@ -2098,7 +2098,7 @@
         <v>1806</v>
       </c>
       <c r="B208" t="n">
-        <v>42945.84411068162</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209">
@@ -2106,7 +2106,7 @@
         <v>1807</v>
       </c>
       <c r="B209" t="n">
-        <v>43327.54419388383</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210">
@@ -2114,7 +2114,7 @@
         <v>1808</v>
       </c>
       <c r="B210" t="n">
-        <v>43718.48476483109</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211">
@@ -2122,7 +2122,7 @@
         <v>1809</v>
       </c>
       <c r="B211" t="n">
-        <v>44118.87879492789</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212">
@@ -2130,7 +2130,7 @@
         <v>1810</v>
       </c>
       <c r="B212" t="n">
-        <v>44528.93545614866</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213">
@@ -2138,7 +2138,7 @@
         <v>1811</v>
       </c>
       <c r="B213" t="n">
-        <v>44948.86014485227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214">
@@ -2146,7 +2146,7 @@
         <v>1812</v>
       </c>
       <c r="B214" t="n">
-        <v>45378.85452355091</v>
+        <v>0</v>
       </c>
     </row>
     <row r="215">
@@ -2154,7 +2154,7 @@
         <v>1813</v>
       </c>
       <c r="B215" t="n">
-        <v>45819.1165803628</v>
+        <v>0</v>
       </c>
     </row>
     <row r="216">
@@ -2162,7 +2162,7 @@
         <v>1814</v>
       </c>
       <c r="B216" t="n">
-        <v>46269.84070577335</v>
+        <v>0</v>
       </c>
     </row>
     <row r="217">
@@ -2170,7 +2170,7 @@
         <v>1815</v>
       </c>
       <c r="B217" t="n">
-        <v>46731.2177863709</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218">
@@ -2178,7 +2178,7 @@
         <v>1816</v>
       </c>
       <c r="B218" t="n">
-        <v>47203.4353151457</v>
+        <v>0</v>
       </c>
     </row>
     <row r="219">
@@ -2186,7 +2186,7 @@
         <v>1817</v>
       </c>
       <c r="B219" t="n">
-        <v>47686.67751787908</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220">
@@ -2194,7 +2194,7 @@
         <v>1818</v>
       </c>
       <c r="B220" t="n">
-        <v>48181.12549516825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="221">
@@ -2202,7 +2202,7 @@
         <v>1819</v>
       </c>
       <c r="B221" t="n">
-        <v>48686.95737961208</v>
+        <v>0</v>
       </c>
     </row>
     <row r="222">
@@ -2210,7 +2210,7 @@
         <v>1820</v>
       </c>
       <c r="B222" t="n">
-        <v>49204.34850748607</v>
+        <v>0</v>
       </c>
     </row>
     <row r="223">
@@ -2218,7 +2218,7 @@
         <v>1821</v>
       </c>
       <c r="B223" t="n">
-        <v>49733.47160454138</v>
+        <v>0</v>
       </c>
     </row>
     <row r="224">
@@ -2226,7 +2226,7 @@
         <v>1822</v>
       </c>
       <c r="B224" t="n">
-        <v>50274.49698514093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="225">
@@ -2234,7 +2234,7 @@
         <v>1823</v>
       </c>
       <c r="B225" t="n">
-        <v>50827.59276430238</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226">
@@ -2242,7 +2242,7 @@
         <v>1824</v>
       </c>
       <c r="B226" t="n">
-        <v>51392.92508181572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227">
@@ -2250,7 +2250,7 @@
         <v>1825</v>
       </c>
       <c r="B227" t="n">
-        <v>51970.6583380452</v>
+        <v>0</v>
       </c>
     </row>
     <row r="228">
@@ -2258,7 +2258,7 @@
         <v>1826</v>
       </c>
       <c r="B228" t="n">
-        <v>52560.9554404986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="229">
@@ -2266,7 +2266,7 @@
         <v>1827</v>
       </c>
       <c r="B229" t="n">
-        <v>53163.97806067537</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230">
@@ -2274,7 +2274,7 @@
         <v>1828</v>
       </c>
       <c r="B230" t="n">
-        <v>53779.88690041877</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231">
@@ -2282,7 +2282,7 @@
         <v>1829</v>
       </c>
       <c r="B231" t="n">
-        <v>54408.84196715503</v>
+        <v>0</v>
       </c>
     </row>
     <row r="232">
@@ -2290,7 +2290,7 @@
         <v>1830</v>
       </c>
       <c r="B232" t="n">
-        <v>55051.00285721081</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233">
@@ -2298,7 +2298,7 @@
         <v>1831</v>
       </c>
       <c r="B233" t="n">
-        <v>55706.52904662879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="234">
@@ -2306,7 +2306,7 @@
         <v>1832</v>
       </c>
       <c r="B234" t="n">
-        <v>56375.58018873424</v>
+        <v>0</v>
       </c>
     </row>
     <row r="235">
@@ -2314,7 +2314,7 @@
         <v>1833</v>
       </c>
       <c r="B235" t="n">
-        <v>57058.31641768871</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236">
@@ -2322,7 +2322,7 @@
         <v>1834</v>
       </c>
       <c r="B236" t="n">
-        <v>57754.89865743324</v>
+        <v>0</v>
       </c>
     </row>
     <row r="237">
@@ -2330,7 +2330,7 @@
         <v>1835</v>
       </c>
       <c r="B237" t="n">
-        <v>58465.48893523009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238">
@@ -2338,7 +2338,7 @@
         <v>1836</v>
       </c>
       <c r="B238" t="n">
-        <v>59190.2506991303</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239">
@@ -2346,7 +2346,7 @@
         <v>1837</v>
       </c>
       <c r="B239" t="n">
-        <v>59929.34913868793</v>
+        <v>0</v>
       </c>
     </row>
     <row r="240">
@@ -2354,7 +2354,7 @@
         <v>1838</v>
       </c>
       <c r="B240" t="n">
-        <v>60682.95150819934</v>
+        <v>0</v>
       </c>
     </row>
     <row r="241">
@@ -2362,7 +2362,7 @@
         <v>1839</v>
       </c>
       <c r="B241" t="n">
-        <v>61451.22745174955</v>
+        <v>0</v>
       </c>
     </row>
     <row r="242">
@@ -2370,7 +2370,7 @@
         <v>1840</v>
       </c>
       <c r="B242" t="n">
-        <v>62234.3493294679</v>
+        <v>0</v>
       </c>
     </row>
     <row r="243">
@@ -2378,7 +2378,7 @@
         <v>1841</v>
       </c>
       <c r="B243" t="n">
-        <v>63032.49254421426</v>
+        <v>0</v>
       </c>
     </row>
     <row r="244">
@@ -2386,7 +2386,7 @@
         <v>1842</v>
       </c>
       <c r="B244" t="n">
-        <v>63845.83586804037</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245">
@@ -2394,7 +2394,7 @@
         <v>1843</v>
       </c>
       <c r="B245" t="n">
-        <v>64674.56176781934</v>
+        <v>0</v>
       </c>
     </row>
     <row r="246">
@@ -2402,7 +2402,7 @@
         <v>1844</v>
       </c>
       <c r="B246" t="n">
-        <v>65518.85672925906</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247">
@@ -2410,7 +2410,7 @@
         <v>1845</v>
       </c>
       <c r="B247" t="n">
-        <v>66378.911578752</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248">
@@ -2418,7 +2418,7 @@
         <v>1846</v>
       </c>
       <c r="B248" t="n">
-        <v>67254.92180230621</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249">
@@ -2426,7 +2426,7 @@
         <v>1847</v>
       </c>
       <c r="B249" t="n">
-        <v>68147.08786094903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250">
@@ -2434,7 +2434,7 @@
         <v>1848</v>
       </c>
       <c r="B250" t="n">
-        <v>69055.61550192935</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251">
@@ -2442,7 +2442,7 @@
         <v>1849</v>
       </c>
       <c r="B251" t="n">
-        <v>69980.7160650859</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252">
@@ -2450,7 +2450,7 @@
         <v>1850</v>
       </c>
       <c r="B252" t="n">
-        <v>70922.60678365979</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253">
@@ -2458,7 +2458,7 @@
         <v>1851</v>
       </c>
       <c r="B253" t="n">
-        <v>71881.51107899587</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254">
@@ -2466,7 +2466,7 @@
         <v>1852</v>
       </c>
       <c r="B254" t="n">
-        <v>72857.65884840448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255">
@@ -2474,7 +2474,7 @@
         <v>1853</v>
       </c>
       <c r="B255" t="n">
-        <v>73851.28674550093</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256">
@@ -2482,7 +2482,7 @@
         <v>1854</v>
       </c>
       <c r="B256" t="n">
-        <v>74862.63845244508</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257">
@@ -2490,7 +2490,7 @@
         <v>1855</v>
       </c>
       <c r="B257" t="n">
-        <v>75891.96494334411</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258">
@@ -2498,7 +2498,7 @@
         <v>1856</v>
       </c>
       <c r="B258" t="n">
-        <v>76939.5247381329</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259">
@@ -2506,7 +2506,7 @@
         <v>1857</v>
       </c>
       <c r="B259" t="n">
-        <v>78005.58414627015</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260">
@@ -2514,7 +2514,7 @@
         <v>1858</v>
       </c>
       <c r="B260" t="n">
-        <v>79090.4174995842</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261">
@@ -2522,7 +2522,7 @@
         <v>1859</v>
       </c>
       <c r="B261" t="n">
-        <v>80194.30737343997</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262">
@@ -2530,7 +2530,7 @@
         <v>1860</v>
       </c>
       <c r="B262" t="n">
-        <v>81317.54479567916</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263">
@@ -2538,7 +2538,7 @@
         <v>1861</v>
       </c>
       <c r="B263" t="n">
-        <v>82460.42944241903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264">
@@ -2546,7 +2546,7 @@
         <v>1862</v>
       </c>
       <c r="B264" t="n">
-        <v>83623.26982003468</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265">
@@ -2554,7 +2554,7 @@
         <v>1863</v>
       </c>
       <c r="B265" t="n">
-        <v>84806.38343266108</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266">
@@ -2562,7 +2562,7 @@
         <v>1864</v>
       </c>
       <c r="B266" t="n">
-        <v>86010.09693410881</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267">
@@ -2570,7 +2570,7 @@
         <v>1865</v>
       </c>
       <c r="B267" t="n">
-        <v>87234.74626378037</v>
+        <v>0</v>
       </c>
     </row>
     <row r="268">
@@ -2578,7 +2578,7 @@
         <v>1866</v>
       </c>
       <c r="B268" t="n">
-        <v>88480.67676545557</v>
+        <v>0</v>
       </c>
     </row>
     <row r="269">
@@ -2586,7 +2586,7 @@
         <v>1867</v>
       </c>
       <c r="B269" t="n">
-        <v>89748.24328816251</v>
+        <v>0</v>
       </c>
     </row>
     <row r="270">
@@ -2594,7 +2594,7 @@
         <v>1868</v>
       </c>
       <c r="B270" t="n">
-        <v>91037.81026834961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="271">
@@ -2602,7 +2602,7 @@
         <v>1869</v>
       </c>
       <c r="B271" t="n">
-        <v>92349.75179230055</v>
+        <v>0</v>
       </c>
     </row>
     <row r="272">
@@ -2610,7 +2610,7 @@
         <v>1870</v>
       </c>
       <c r="B272" t="n">
-        <v>93684.4516380042</v>
+        <v>0</v>
       </c>
     </row>
     <row r="273">
@@ -2618,7 +2618,7 @@
         <v>1871</v>
       </c>
       <c r="B273" t="n">
-        <v>95042.30329538314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="274">
@@ -2626,7 +2626,7 @@
         <v>1872</v>
       </c>
       <c r="B274" t="n">
-        <v>96423.70996400365</v>
+        <v>0</v>
       </c>
     </row>
     <row r="275">
@@ -2634,7 +2634,7 @@
         <v>1873</v>
       </c>
       <c r="B275" t="n">
-        <v>97829.0845272061</v>
+        <v>0</v>
       </c>
     </row>
     <row r="276">
@@ -2642,7 +2642,7 @@
         <v>1874</v>
       </c>
       <c r="B276" t="n">
-        <v>99258.84950158122</v>
+        <v>0</v>
       </c>
     </row>
     <row r="277">
@@ -2650,7 +2650,7 @@
         <v>1875</v>
       </c>
       <c r="B277" t="n">
-        <v>100713.4369608227</v>
+        <v>0</v>
       </c>
     </row>
     <row r="278">
@@ -2658,7 +2658,7 @@
         <v>1876</v>
       </c>
       <c r="B278" t="n">
-        <v>102193.2884327507</v>
+        <v>0</v>
       </c>
     </row>
     <row r="279">
@@ -2666,7 +2666,7 @@
         <v>1877</v>
       </c>
       <c r="B279" t="n">
-        <v>103698.8547684665</v>
+        <v>0</v>
       </c>
     </row>
     <row r="280">
@@ -2674,7 +2674,7 @@
         <v>1878</v>
       </c>
       <c r="B280" t="n">
-        <v>105230.5959824378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="281">
@@ -2682,7 +2682,7 @@
         <v>1879</v>
       </c>
       <c r="B281" t="n">
-        <v>106788.9810624047</v>
+        <v>0</v>
       </c>
     </row>
     <row r="282">
@@ -2690,7 +2690,7 @@
         <v>1880</v>
       </c>
       <c r="B282" t="n">
-        <v>108374.4877478575</v>
+        <v>0</v>
       </c>
     </row>
     <row r="283">
@@ -2698,7 +2698,7 @@
         <v>1881</v>
       </c>
       <c r="B283" t="n">
-        <v>109987.602275917</v>
+        <v>0</v>
       </c>
     </row>
     <row r="284">
@@ -2706,7 +2706,7 @@
         <v>1882</v>
       </c>
       <c r="B284" t="n">
-        <v>111628.8190933637</v>
+        <v>0</v>
       </c>
     </row>
     <row r="285">
@@ -2714,7 +2714,7 @@
         <v>1883</v>
       </c>
       <c r="B285" t="n">
-        <v>113298.6405335878</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286">
@@ -2722,7 +2722,7 @@
         <v>1884</v>
       </c>
       <c r="B286" t="n">
-        <v>114997.5764572338</v>
+        <v>0</v>
       </c>
     </row>
     <row r="287">
@@ -2730,7 +2730,7 @@
         <v>1885</v>
       </c>
       <c r="B287" t="n">
-        <v>116726.1438551658</v>
+        <v>0</v>
       </c>
     </row>
     <row r="288">
@@ -2738,7 +2738,7 @@
         <v>1886</v>
       </c>
       <c r="B288" t="n">
-        <v>118484.8664126494</v>
+        <v>0</v>
       </c>
     </row>
     <row r="289">
@@ -2746,7 +2746,7 @@
         <v>1887</v>
       </c>
       <c r="B289" t="n">
-        <v>120274.2740333408</v>
+        <v>0</v>
       </c>
     </row>
     <row r="290">
@@ -2754,7 +2754,7 @@
         <v>1888</v>
       </c>
       <c r="B290" t="n">
-        <v>122094.902321903</v>
+        <v>0</v>
       </c>
     </row>
     <row r="291">
@@ -2762,7 +2762,7 @@
         <v>1889</v>
       </c>
       <c r="B291" t="n">
-        <v>123947.2920239631</v>
+        <v>0</v>
       </c>
     </row>
     <row r="292">
@@ -2770,7 +2770,7 @@
         <v>1890</v>
       </c>
       <c r="B292" t="n">
-        <v>125831.9884221626</v>
+        <v>0</v>
       </c>
     </row>
     <row r="293">
@@ -2778,7 +2778,7 @@
         <v>1891</v>
       </c>
       <c r="B293" t="n">
-        <v>127749.5406870961</v>
+        <v>0</v>
       </c>
     </row>
     <row r="294">
@@ -2786,7 +2786,7 @@
         <v>1892</v>
       </c>
       <c r="B294" t="n">
-        <v>129700.5011820242</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295">
@@ -2794,7 +2794,7 @@
         <v>1893</v>
       </c>
       <c r="B295" t="n">
-        <v>131685.4247200091</v>
+        <v>0</v>
       </c>
     </row>
     <row r="296">
@@ -2802,7 +2802,7 @@
         <v>1894</v>
       </c>
       <c r="B296" t="n">
-        <v>133704.8677726211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="297">
@@ -2810,7 +2810,7 @@
         <v>1895</v>
       </c>
       <c r="B297" t="n">
-        <v>135759.387628992</v>
+        <v>0</v>
       </c>
     </row>
     <row r="298">
@@ -2818,7 +2818,7 @@
         <v>1896</v>
       </c>
       <c r="B298" t="n">
-        <v>137849.5415042592</v>
+        <v>0</v>
       </c>
     </row>
     <row r="299">
@@ -2826,7 +2826,7 @@
         <v>1897</v>
       </c>
       <c r="B299" t="n">
-        <v>139975.8855964843</v>
+        <v>0</v>
       </c>
     </row>
     <row r="300">
@@ -2834,7 +2834,7 @@
         <v>1898</v>
       </c>
       <c r="B300" t="n">
-        <v>142138.9740912785</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301">
@@ -2842,7 +2842,7 @@
         <v>1899</v>
       </c>
       <c r="B301" t="n">
-        <v>144339.3581132782</v>
+        <v>0</v>
       </c>
     </row>
     <row r="302">
@@ -2850,7 +2850,7 @@
         <v>1900</v>
       </c>
       <c r="B302" t="n">
-        <v>146577.5846238236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303">

</xml_diff>

<commit_message>
calibration is done. scenario run modeling of renovation changes started
</commit_message>
<xml_diff>
--- a/Data/model_outputs_baseline/UFA/i_AB_UFA.xlsx
+++ b/Data/model_outputs_baseline/UFA/i_AB_UFA.xlsx
@@ -2858,7 +2858,7 @@
         <v>1901</v>
       </c>
       <c r="B303" t="n">
-        <v>148854.1952645268</v>
+        <v>87504.31089811739</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>1902</v>
       </c>
       <c r="B304" t="n">
-        <v>151169.7251460525</v>
+        <v>88893.57453918592</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>1903</v>
       </c>
       <c r="B305" t="n">
-        <v>153524.7015819957</v>
+        <v>90306.91963708345</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>1904</v>
       </c>
       <c r="B306" t="n">
-        <v>155919.6427678394</v>
+        <v>91744.67394044143</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>1905</v>
       </c>
       <c r="B307" t="n">
-        <v>158355.0564049098</v>
+        <v>93207.1594356229</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>1906</v>
       </c>
       <c r="B308" t="n">
-        <v>160831.4382696307</v>
+        <v>94694.69149521155</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>1907</v>
       </c>
       <c r="B309" t="n">
-        <v>163349.2707286709</v>
+        <v>96207.57799301714</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>1908</v>
       </c>
       <c r="B310" t="n">
-        <v>165909.0212005182</v>
+        <v>97746.11838583663</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>1909</v>
       </c>
       <c r="B311" t="n">
-        <v>168511.1405643169</v>
+        <v>99310.60276239192</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>1910</v>
       </c>
       <c r="B312" t="n">
-        <v>171156.0615173977</v>
+        <v>100901.3108602124</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>1911</v>
       </c>
       <c r="B313" t="n">
-        <v>173844.1968827201</v>
+        <v>102518.5110511117</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>1912</v>
       </c>
       <c r="B314" t="n">
-        <v>176575.9378678495</v>
+        <v>104162.4592961455</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>1913</v>
       </c>
       <c r="B315" t="n">
-        <v>179351.6522777024</v>
+        <v>105833.3980713008</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>1914</v>
       </c>
       <c r="B316" t="n">
-        <v>182171.6826832094</v>
+        <v>107531.55526512</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>1915</v>
       </c>
       <c r="B317" t="n">
-        <v>185036.3445484739</v>
+        <v>109257.1430497207</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>1916</v>
       </c>
       <c r="B318" t="n">
-        <v>187945.924319636</v>
+        <v>111010.356727047</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>1917</v>
       </c>
       <c r="B319" t="n">
-        <v>190900.677478451</v>
+        <v>112791.3735520751</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>1918</v>
       </c>
       <c r="B320" t="n">
-        <v>193900.8265644546</v>
+        <v>114600.3515352117</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>1919</v>
       </c>
       <c r="B321" t="n">
-        <v>196946.5591699187</v>
+        <v>116437.4282263228</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>1920</v>
       </c>
       <c r="B322" t="n">
-        <v>200038.0259116633</v>
+        <v>118302.7194827578</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>1921</v>
       </c>
       <c r="B323" t="n">
-        <v>203175.3383850391</v>
+        <v>120196.3182244761</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>1922</v>
       </c>
       <c r="B324" t="n">
-        <v>206358.5671048734</v>
+        <v>122118.2931790851</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>1923</v>
       </c>
       <c r="B325" t="n">
-        <v>209587.739439592</v>
+        <v>124068.6876204429</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>1924</v>
       </c>
       <c r="B326" t="n">
-        <v>212862.8375440528</v>
+        <v>126047.5181040914</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>1925</v>
       </c>
       <c r="B327" t="n">
-        <v>216183.7962979455</v>
+        <v>128054.7732035716</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>1926</v>
       </c>
       <c r="B328" t="n">
-        <v>219550.5012566099</v>
+        <v>130090.4122516834</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>1927</v>
       </c>
       <c r="B329" t="n">
-        <v>222962.7866214565</v>
+        <v>132154.36409096</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>1928</v>
       </c>
       <c r="B330" t="n">
-        <v>226420.4332378391</v>
+        <v>134246.5258380295</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>1929</v>
       </c>
       <c r="B331" t="n">
-        <v>229923.1666284592</v>
+        <v>136366.7616666898</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>1930</v>
       </c>
       <c r="B332" t="n">
-        <v>233470.6550708087</v>
+        <v>138514.9016147816</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>1931</v>
       </c>
       <c r="B333" t="n">
-        <v>237062.507727374</v>
+        <v>140690.7404200932</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>1932</v>
       </c>
       <c r="B334" t="n">
-        <v>240698.2728380108</v>
+        <v>142894.0363909452</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>1933</v>
       </c>
       <c r="B335" t="n">
-        <v>244377.435983801</v>
+        <v>145124.5103170638</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>1934</v>
       </c>
       <c r="B336" t="n">
-        <v>248099.4184322895</v>
+        <v>147381.844426711</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>1935</v>
       </c>
       <c r="B337" t="n">
-        <v>251863.5755742106</v>
+        <v>149665.681396185</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>1936</v>
       </c>
       <c r="B338" t="n">
-        <v>255669.19546188</v>
+        <v>151975.6234178527</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>1937</v>
       </c>
       <c r="B339" t="n">
-        <v>259515.4974597098</v>
+        <v>154311.2313330686</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>1938</v>
       </c>
       <c r="B340" t="n">
-        <v>263401.6310178202</v>
+        <v>156672.0238366463</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>1939</v>
       </c>
       <c r="B341" t="n">
-        <v>267326.6745790193</v>
+        <v>159057.4767591608</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>1940</v>
       </c>
       <c r="B342" t="n">
-        <v>271289.6346302294</v>
+        <v>161467.0224338428</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>1941</v>
       </c>
       <c r="B343" t="n">
-        <v>275289.4449092285</v>
+        <v>163900.0491547308</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>1942</v>
       </c>
       <c r="B344" t="n">
-        <v>279324.965777263</v>
+        <v>166355.9007325691</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>1943</v>
       </c>
       <c r="B345" t="n">
-        <v>283394.983768516</v>
+        <v>168833.8761552153</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>1944</v>
       </c>
       <c r="B346" t="n">
-        <v>287498.2113264588</v>
+        <v>171333.2293587682</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>1945</v>
       </c>
       <c r="B347" t="n">
-        <v>291633.2867381297</v>
+        <v>173853.1691162469</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>1946</v>
       </c>
       <c r="B348" t="n">
-        <v>295798.7742754684</v>
+        <v>176392.8590495294</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>1947</v>
       </c>
       <c r="B349" t="n">
-        <v>299993.1645542902</v>
+        <v>178951.4177711401</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>1948</v>
       </c>
       <c r="B350" t="n">
-        <v>304214.8751192529</v>
+        <v>181527.9191611617</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>1949</v>
       </c>
       <c r="B351" t="n">
-        <v>308462.2512644377</v>
+        <v>184121.3927853182</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>1950</v>
       </c>
       <c r="B352" t="n">
-        <v>312733.567097062</v>
+        <v>186730.8244590356</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>1951</v>
       </c>
       <c r="B353" t="n">
-        <v>317027.0268524086</v>
+        <v>189355.1569626348</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>1952</v>
       </c>
       <c r="B354" t="n">
-        <v>321340.7664664974</v>
+        <v>191993.2909118975</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>1953</v>
       </c>
       <c r="B355" t="n">
-        <v>325672.8554129532</v>
+        <v>194644.0857882107</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>1954</v>
       </c>
       <c r="B356" t="n">
-        <v>330021.2988091259</v>
+        <v>197306.3611316709</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>1955</v>
       </c>
       <c r="B357" t="n">
-        <v>334384.0397959869</v>
+        <v>199978.8979002218</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>1956</v>
       </c>
       <c r="B358" t="n">
-        <v>384702.4420640444</v>
+        <v>217816.5993111332</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>1957</v>
       </c>
       <c r="B359" t="n">
-        <v>389682.0704982577</v>
+        <v>220706.9739227913</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>1958</v>
       </c>
       <c r="B360" t="n">
-        <v>394670.5376285968</v>
+        <v>223604.2152717551</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>1959</v>
       </c>
       <c r="B361" t="n">
-        <v>399665.2594679759</v>
+        <v>226506.8655326307</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>1960</v>
       </c>
       <c r="B362" t="n">
-        <v>404663.5999190195</v>
+        <v>229413.4354609017</v>
       </c>
     </row>
     <row r="363">
@@ -3338,7 +3338,7 @@
         <v>1961</v>
       </c>
       <c r="B363" t="n">
-        <v>409662.8753810604</v>
+        <v>232322.4069550165</v>
       </c>
     </row>
     <row r="364">
@@ -3346,7 +3346,7 @@
         <v>1962</v>
       </c>
       <c r="B364" t="n">
-        <v>414660.3596694295</v>
+        <v>235232.2358005846</v>
       </c>
     </row>
     <row r="365">
@@ -3354,7 +3354,7 @@
         <v>1963</v>
       </c>
       <c r="B365" t="n">
-        <v>419653.2892407456</v>
+        <v>238141.3545935237</v>
       </c>
     </row>
     <row r="366">
@@ -3362,7 +3362,7 @@
         <v>1964</v>
       </c>
       <c r="B366" t="n">
-        <v>424638.8687177499</v>
+        <v>241048.1758388956</v>
       </c>
     </row>
     <row r="367">
@@ -3370,7 +3370,7 @@
         <v>1965</v>
       </c>
       <c r="B367" t="n">
-        <v>429614.276705681</v>
+        <v>243951.0952212831</v>
       </c>
     </row>
     <row r="368">
@@ -3378,7 +3378,7 @@
         <v>1966</v>
       </c>
       <c r="B368" t="n">
-        <v>434576.6718893859</v>
+        <v>246848.4950409575</v>
       </c>
     </row>
     <row r="369">
@@ -3386,7 +3386,7 @@
         <v>1967</v>
       </c>
       <c r="B369" t="n">
-        <v>439523.1994009324</v>
+        <v>249738.7478103951</v>
       </c>
     </row>
     <row r="370">
@@ -3394,7 +3394,7 @@
         <v>1968</v>
       </c>
       <c r="B370" t="n">
-        <v>444450.9974437963</v>
+        <v>252620.2200035911</v>
       </c>
     </row>
     <row r="371">
@@ -3402,7 +3402,7 @@
         <v>1969</v>
       </c>
       <c r="B371" t="n">
-        <v>449357.2041599904</v>
+        <v>255491.2759507617</v>
       </c>
     </row>
     <row r="372">
@@ -3410,7 +3410,7 @@
         <v>1970</v>
       </c>
       <c r="B372" t="n">
-        <v>454238.9647242792</v>
+        <v>258350.2818697478</v>
       </c>
     </row>
     <row r="373">
@@ -3418,7 +3418,7 @@
         <v>1971</v>
       </c>
       <c r="B373" t="n">
-        <v>388329.3519588731</v>
+        <v>254283.9628051224</v>
       </c>
     </row>
     <row r="374">
@@ -3426,7 +3426,7 @@
         <v>1972</v>
       </c>
       <c r="B374" t="n">
-        <v>392410.0984573025</v>
+        <v>257039.1086512413</v>
       </c>
     </row>
     <row r="375">
@@ -3434,7 +3434,7 @@
         <v>1973</v>
       </c>
       <c r="B375" t="n">
-        <v>396463.0208102779</v>
+        <v>259777.8037519292</v>
       </c>
     </row>
     <row r="376">
@@ -3442,7 +3442,7 @@
         <v>1974</v>
       </c>
       <c r="B376" t="n">
-        <v>400485.791341435</v>
+        <v>262498.5064773588</v>
       </c>
     </row>
     <row r="377">
@@ -3450,7 +3450,7 @@
         <v>1975</v>
       </c>
       <c r="B377" t="n">
-        <v>404476.120660253</v>
+        <v>265199.6983062237</v>
       </c>
     </row>
     <row r="378">
@@ -3458,7 +3458,7 @@
         <v>1976</v>
       </c>
       <c r="B378" t="n">
-        <v>408431.7644728207</v>
+        <v>267879.8883301202</v>
       </c>
     </row>
     <row r="379">
@@ -3466,7 +3466,7 @@
         <v>1977</v>
       </c>
       <c r="B379" t="n">
-        <v>412350.530461649</v>
+        <v>270537.6178119734</v>
       </c>
     </row>
     <row r="380">
@@ -3474,7 +3474,7 @@
         <v>1978</v>
       </c>
       <c r="B380" t="n">
-        <v>416230.2852135569</v>
+        <v>273171.4647848681</v>
       </c>
     </row>
     <row r="381">
@@ -3482,7 +3482,7 @@
         <v>1979</v>
       </c>
       <c r="B381" t="n">
-        <v>420068.961174161</v>
+        <v>275780.048677278</v>
       </c>
     </row>
     <row r="382">
@@ -3490,7 +3490,7 @@
         <v>1980</v>
       </c>
       <c r="B382" t="n">
-        <v>423864.563606775</v>
+        <v>278362.0349501816</v>
       </c>
     </row>
     <row r="383">
@@ -3498,7 +3498,7 @@
         <v>1981</v>
       </c>
       <c r="B383" t="n">
-        <v>312278.6486173721</v>
+        <v>215236.5443044131</v>
       </c>
     </row>
     <row r="384">
@@ -3506,7 +3506,7 @@
         <v>1982</v>
       </c>
       <c r="B384" t="n">
-        <v>314983.4561514351</v>
+        <v>217171.1826432301</v>
       </c>
     </row>
     <row r="385">
@@ -3514,7 +3514,7 @@
         <v>1983</v>
       </c>
       <c r="B385" t="n">
-        <v>317652.807407144</v>
+        <v>219082.6215159229</v>
       </c>
     </row>
     <row r="386">
@@ -3522,7 +3522,7 @@
         <v>1984</v>
       </c>
       <c r="B386" t="n">
-        <v>320285.5086866005</v>
+        <v>220970.0147998908</v>
       </c>
     </row>
     <row r="387">
@@ -3530,7 +3530,7 @@
         <v>1985</v>
       </c>
       <c r="B387" t="n">
-        <v>322880.4443492013</v>
+        <v>222832.5691449723</v>
       </c>
     </row>
     <row r="388">
@@ -3538,7 +3538,7 @@
         <v>1986</v>
       </c>
       <c r="B388" t="n">
-        <v>325436.5815644222</v>
+        <v>224669.5473402231</v>
       </c>
     </row>
     <row r="389">
@@ -3546,7 +3546,7 @@
         <v>1987</v>
       </c>
       <c r="B389" t="n">
-        <v>327952.9749512962</v>
+        <v>226480.2716090042</v>
       </c>
     </row>
     <row r="390">
@@ -3554,7 +3554,7 @@
         <v>1988</v>
       </c>
       <c r="B390" t="n">
-        <v>330428.771088318</v>
+        <v>228264.1268209793</v>
       </c>
     </row>
     <row r="391">
@@ -3562,7 +3562,7 @@
         <v>1989</v>
       </c>
       <c r="B391" t="n">
-        <v>332863.2128775233</v>
+        <v>230020.5636096019</v>
       </c>
     </row>
     <row r="392">
@@ -3570,7 +3570,7 @@
         <v>1990</v>
       </c>
       <c r="B392" t="n">
-        <v>335255.6437472118</v>
+        <v>231749.1013841411</v>
       </c>
     </row>
     <row r="393">
@@ -3578,7 +3578,7 @@
         <v>1991</v>
       </c>
       <c r="B393" t="n">
-        <v>547933.7569709384</v>
+        <v>343367.4969921544</v>
       </c>
     </row>
     <row r="394">
@@ -3586,7 +3586,7 @@
         <v>1992</v>
       </c>
       <c r="B394" t="n">
-        <v>551677.7930325336</v>
+        <v>345826.1409646957</v>
       </c>
     </row>
     <row r="395">
@@ -3594,7 +3594,7 @@
         <v>1993</v>
       </c>
       <c r="B395" t="n">
-        <v>555351.4912048004</v>
+        <v>348242.2778140905</v>
       </c>
     </row>
     <row r="396">
@@ -3602,7 +3602,7 @@
         <v>1994</v>
       </c>
       <c r="B396" t="n">
-        <v>558954.5005958162</v>
+        <v>350615.645944871</v>
       </c>
     </row>
     <row r="397">
@@ -3610,7 +3610,7 @@
         <v>1995</v>
       </c>
       <c r="B397" t="n">
-        <v>562486.662791495</v>
+        <v>352946.1041959572</v>
       </c>
     </row>
     <row r="398">
@@ -3618,7 +3618,7 @@
         <v>1996</v>
       </c>
       <c r="B398" t="n">
-        <v>565948.016604474</v>
+        <v>355233.6350174868</v>
       </c>
     </row>
     <row r="399">
@@ -3626,7 +3626,7 @@
         <v>1997</v>
       </c>
       <c r="B399" t="n">
-        <v>569338.8024019549</v>
+        <v>357478.3473894878</v>
       </c>
     </row>
     <row r="400">
@@ -3634,7 +3634,7 @@
         <v>1998</v>
       </c>
       <c r="B400" t="n">
-        <v>572659.4659918119</v>
+        <v>359680.4794688068</v>
       </c>
     </row>
     <row r="401">
@@ -3642,7 +3642,7 @@
         <v>1999</v>
       </c>
       <c r="B401" t="n">
-        <v>575910.6620495005</v>
+        <v>361840.4009527031</v>
       </c>
     </row>
     <row r="402">
@@ -3650,7 +3650,7 @@
         <v>2000</v>
       </c>
       <c r="B402" t="n">
-        <v>579093.257065926</v>
+        <v>363958.6151459903</v>
       </c>
     </row>
     <row r="403">
@@ -3658,7 +3658,7 @@
         <v>2001</v>
       </c>
       <c r="B403" t="n">
-        <v>892259.3841081732</v>
+        <v>983043.8436066696</v>
       </c>
     </row>
     <row r="404">
@@ -3666,7 +3666,7 @@
         <v>2002</v>
       </c>
       <c r="B404" t="n">
-        <v>896931.8804306486</v>
+        <v>988514.1158130482</v>
       </c>
     </row>
     <row r="405">
@@ -3674,7 +3674,7 @@
         <v>2003</v>
       </c>
       <c r="B405" t="n">
-        <v>901505.2078331888</v>
+        <v>993878.6278342606</v>
       </c>
     </row>
     <row r="406">
@@ -3682,7 +3682,7 @@
         <v>2004</v>
       </c>
       <c r="B406" t="n">
-        <v>905982.0223192225</v>
+        <v>999140.2052091751</v>
       </c>
     </row>
     <row r="407">
@@ -3690,7 +3690,7 @@
         <v>2005</v>
       </c>
       <c r="B407" t="n">
-        <v>910365.3151948994</v>
+        <v>1004302.047068411</v>
       </c>
     </row>
     <row r="408">
@@ -3698,7 +3698,7 @@
         <v>2006</v>
       </c>
       <c r="B408" t="n">
-        <v>914658.4126515005</v>
+        <v>1009367.726283663</v>
       </c>
     </row>
     <row r="409">
@@ -3706,7 +3706,7 @@
         <v>2007</v>
       </c>
       <c r="B409" t="n">
-        <v>918864.9744423676</v>
+        <v>1014341.188617754</v>
       </c>
     </row>
     <row r="410">
@@ -3714,7 +3714,7 @@
         <v>2008</v>
       </c>
       <c r="B410" t="n">
-        <v>922988.9916271614</v>
+        <v>1019226.750843105</v>
       </c>
     </row>
     <row r="411">
@@ -3722,7 +3722,7 @@
         <v>2009</v>
       </c>
       <c r="B411" t="n">
-        <v>927034.7833638517</v>
+        <v>1024029.097804603</v>
       </c>
     </row>
     <row r="412">
@@ -3730,7 +3730,7 @@
         <v>2010</v>
       </c>
       <c r="B412" t="n">
-        <v>931006.9927205181</v>
+        <v>1028753.278393618</v>
       </c>
     </row>
     <row r="413">
@@ -3738,7 +3738,7 @@
         <v>2011</v>
       </c>
       <c r="B413" t="n">
-        <v>890521.1060350555</v>
+        <v>1115583.896842943</v>
       </c>
     </row>
     <row r="414">
@@ -3746,7 +3746,7 @@
         <v>2012</v>
       </c>
       <c r="B414" t="n">
-        <v>894179.0141122377</v>
+        <v>1120532.886744793</v>
       </c>
     </row>
     <row r="415">
@@ -3754,7 +3754,7 @@
         <v>2013</v>
       </c>
       <c r="B415" t="n">
-        <v>897781.8981732667</v>
+        <v>1125416.141705901</v>
       </c>
     </row>
     <row r="416">
@@ -3762,7 +3762,7 @@
         <v>2014</v>
       </c>
       <c r="B416" t="n">
-        <v>901335.3556099772</v>
+        <v>1130240.616060636</v>
       </c>
     </row>
     <row r="417">
@@ -3770,7 +3770,7 @@
         <v>2015</v>
       </c>
       <c r="B417" t="n">
-        <v>904845.2575909977</v>
+        <v>1135013.616674762</v>
       </c>
     </row>
     <row r="418">
@@ -3778,7 +3778,7 @@
         <v>2016</v>
       </c>
       <c r="B418" t="n">
-        <v>908317.7389730286</v>
+        <v>1139742.790863914</v>
       </c>
     </row>
     <row r="419">
@@ -3786,7 +3786,7 @@
         <v>2017</v>
       </c>
       <c r="B419" t="n">
-        <v>911759.1871051961</v>
+        <v>1144436.112898908</v>
       </c>
     </row>
     <row r="420">
@@ -3794,7 +3794,7 @@
         <v>2018</v>
       </c>
       <c r="B420" t="n">
-        <v>915176.2294984999</v>
+        <v>1149101.869059497</v>
       </c>
     </row>
     <row r="421">
@@ -3802,7 +3802,7 @@
         <v>2019</v>
       </c>
       <c r="B421" t="n">
-        <v>918575.7203331122</v>
+        <v>1153748.641199037</v>
       </c>
     </row>
     <row r="422">
@@ -3810,7 +3810,7 @@
         <v>2020</v>
       </c>
       <c r="B422" t="n">
-        <v>921964.7257744141</v>
+        <v>1158385.28878004</v>
       </c>
     </row>
     <row r="423">
@@ -3818,7 +3818,7 @@
         <v>2021</v>
       </c>
       <c r="B423" t="n">
-        <v>925350.5080720098</v>
+        <v>1163020.929344759</v>
       </c>
     </row>
     <row r="424">
@@ -3826,7 +3826,7 @@
         <v>2022</v>
       </c>
       <c r="B424" t="n">
-        <v>928740.5084118656</v>
+        <v>1167664.917379638</v>
       </c>
     </row>
     <row r="425">
@@ -3834,7 +3834,7 @@
         <v>2023</v>
       </c>
       <c r="B425" t="n">
-        <v>932142.3284982925</v>
+        <v>1172326.821540681</v>
       </c>
     </row>
     <row r="426">
@@ -3842,7 +3842,7 @@
         <v>2024</v>
       </c>
       <c r="B426" t="n">
-        <v>935563.7108377402</v>
+        <v>1177016.400200688</v>
       </c>
     </row>
     <row r="427">
@@ -3850,7 +3850,7 @@
         <v>2025</v>
       </c>
       <c r="B427" t="n">
-        <v>939012.5177038754</v>
+        <v>1181743.575288674</v>
       </c>
     </row>
     <row r="428">
@@ -3858,7 +3858,7 @@
         <v>2026</v>
       </c>
       <c r="B428" t="n">
-        <v>942496.7087630519</v>
+        <v>1186518.404391232</v>
       </c>
     </row>
     <row r="429">
@@ -3866,7 +3866,7 @@
         <v>2027</v>
       </c>
       <c r="B429" t="n">
-        <v>946024.3173423079</v>
+        <v>1191351.05108934</v>
       </c>
     </row>
     <row r="430">
@@ -3874,7 +3874,7 @@
         <v>2028</v>
       </c>
       <c r="B430" t="n">
-        <v>949603.4253287641</v>
+        <v>1196251.753512539</v>
       </c>
     </row>
     <row r="431">
@@ -3882,7 +3882,7 @@
         <v>2029</v>
       </c>
       <c r="B431" t="n">
-        <v>953242.1366917371</v>
+        <v>1201230.791095426</v>
       </c>
     </row>
     <row r="432">
@@ -3890,7 +3890,7 @@
         <v>2030</v>
       </c>
       <c r="B432" t="n">
-        <v>956948.5496256596</v>
+        <v>1206298.449529908</v>
       </c>
     </row>
     <row r="433">
@@ -3898,7 +3898,7 @@
         <v>2031</v>
       </c>
       <c r="B433" t="n">
-        <v>960730.7273203218</v>
+        <v>1211464.983917283</v>
       </c>
     </row>
     <row r="434">
@@ -3906,7 +3906,7 @@
         <v>2032</v>
       </c>
       <c r="B434" t="n">
-        <v>964596.6673699646</v>
+        <v>1216740.580130534</v>
       </c>
     </row>
     <row r="435">
@@ -3914,7 +3914,7 @@
         <v>2033</v>
       </c>
       <c r="B435" t="n">
-        <v>968554.2698457993</v>
+        <v>1222135.314413717</v>
       </c>
     </row>
     <row r="436">
@@ -3922,7 +3922,7 @@
         <v>2034</v>
       </c>
       <c r="B436" t="n">
-        <v>972611.3040619596</v>
+        <v>1227659.111252251</v>
       </c>
     </row>
     <row r="437">
@@ -3930,7 +3930,7 @@
         <v>2035</v>
       </c>
       <c r="B437" t="n">
-        <v>976775.3740820516</v>
+        <v>1233321.699569666</v>
       </c>
     </row>
     <row r="438">
@@ -3938,7 +3938,7 @@
         <v>2036</v>
       </c>
       <c r="B438" t="n">
-        <v>981053.8830199146</v>
+        <v>1239132.567314676</v>
       </c>
     </row>
     <row r="439">
@@ -3946,7 +3946,7 @@
         <v>2037</v>
       </c>
       <c r="B439" t="n">
-        <v>985453.9962081041</v>
+        <v>1245100.914527719</v>
       </c>
     </row>
     <row r="440">
@@ -3954,7 +3954,7 @@
         <v>2038</v>
       </c>
       <c r="B440" t="n">
-        <v>989982.6033164308</v>
+        <v>1251235.60498753</v>
       </c>
     </row>
     <row r="441">
@@ -3962,7 +3962,7 @@
         <v>2039</v>
       </c>
       <c r="B441" t="n">
-        <v>994646.2795243766</v>
+        <v>1257545.116565706</v>
       </c>
     </row>
     <row r="442">
@@ -3970,7 +3970,7 @@
         <v>2040</v>
       </c>
       <c r="B442" t="n">
-        <v>999451.2458644067</v>
+        <v>1264037.490434306</v>
       </c>
     </row>
     <row r="443">
@@ -3978,7 +3978,7 @@
         <v>2041</v>
       </c>
       <c r="B443" t="n">
-        <v>1004403.328871989</v>
+        <v>1270720.279295618</v>
       </c>
     </row>
     <row r="444">
@@ -3986,7 +3986,7 @@
         <v>2042</v>
       </c>
       <c r="B444" t="n">
-        <v>1009507.919698519</v>
+        <v>1277600.494829536</v>
       </c>
     </row>
     <row r="445">
@@ -3994,7 +3994,7 @@
         <v>2043</v>
       </c>
       <c r="B445" t="n">
-        <v>1014769.932860437</v>
+        <v>1284684.554576099</v>
       </c>
     </row>
     <row r="446">
@@ -4002,7 +4002,7 @@
         <v>2044</v>
       </c>
       <c r="B446" t="n">
-        <v>1020193.764819022</v>
+        <v>1291978.228498197</v>
       </c>
     </row>
     <row r="447">
@@ -4010,7 +4010,7 @@
         <v>2045</v>
       </c>
       <c r="B447" t="n">
-        <v>1025783.25260493</v>
+        <v>1299486.585494871</v>
       </c>
     </row>
     <row r="448">
@@ -4018,7 +4018,7 @@
         <v>2046</v>
       </c>
       <c r="B448" t="n">
-        <v>1031541.632722011</v>
+        <v>1307213.94016231</v>
       </c>
     </row>
     <row r="449">
@@ -4026,7 +4026,7 @@
         <v>2047</v>
       </c>
       <c r="B449" t="n">
-        <v>1037471.500586605</v>
+        <v>1315163.800127917</v>
       </c>
     </row>
     <row r="450">
@@ -4034,7 +4034,7 @@
         <v>2048</v>
       </c>
       <c r="B450" t="n">
-        <v>1043574.770772868</v>
+        <v>1323338.814301805</v>
       </c>
     </row>
     <row r="451">
@@ -4042,7 +4042,7 @@
         <v>2049</v>
       </c>
       <c r="B451" t="n">
-        <v>1049852.638361668</v>
+        <v>1331740.722425331</v>
       </c>
     </row>
     <row r="452">
@@ -4050,7 +4050,7 @@
         <v>2050</v>
       </c>
       <c r="B452" t="n">
-        <v>1056305.541701093</v>
+        <v>1340370.306310536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correcting a test made earlier
</commit_message>
<xml_diff>
--- a/Data/model_outputs_baseline/UFA/i_AB_UFA.xlsx
+++ b/Data/model_outputs_baseline/UFA/i_AB_UFA.xlsx
@@ -2858,7 +2858,7 @@
         <v>1901</v>
       </c>
       <c r="B303" t="n">
-        <v>87504.31089811739</v>
+        <v>87504.31089849597</v>
       </c>
     </row>
     <row r="304">
@@ -2866,7 +2866,7 @@
         <v>1902</v>
       </c>
       <c r="B304" t="n">
-        <v>88893.57453918592</v>
+        <v>88893.57453954748</v>
       </c>
     </row>
     <row r="305">
@@ -2874,7 +2874,7 @@
         <v>1903</v>
       </c>
       <c r="B305" t="n">
-        <v>90306.91963708345</v>
+        <v>90306.9196374287</v>
       </c>
     </row>
     <row r="306">
@@ -2882,7 +2882,7 @@
         <v>1904</v>
       </c>
       <c r="B306" t="n">
-        <v>91744.67394044143</v>
+        <v>91744.67394076909</v>
       </c>
     </row>
     <row r="307">
@@ -2890,7 +2890,7 @@
         <v>1905</v>
       </c>
       <c r="B307" t="n">
-        <v>93207.1594356229</v>
+        <v>93207.15943593236</v>
       </c>
     </row>
     <row r="308">
@@ -2898,7 +2898,7 @@
         <v>1906</v>
       </c>
       <c r="B308" t="n">
-        <v>94694.69149521155</v>
+        <v>94694.69149550417</v>
       </c>
     </row>
     <row r="309">
@@ -2906,7 +2906,7 @@
         <v>1907</v>
       </c>
       <c r="B309" t="n">
-        <v>96207.57799301714</v>
+        <v>96207.57799329038</v>
       </c>
     </row>
     <row r="310">
@@ -2914,7 +2914,7 @@
         <v>1908</v>
       </c>
       <c r="B310" t="n">
-        <v>97746.11838583663</v>
+        <v>97746.11838608925</v>
       </c>
     </row>
     <row r="311">
@@ -2922,7 +2922,7 @@
         <v>1909</v>
       </c>
       <c r="B311" t="n">
-        <v>99310.60276239192</v>
+        <v>99310.60276262525</v>
       </c>
     </row>
     <row r="312">
@@ -2930,7 +2930,7 @@
         <v>1910</v>
       </c>
       <c r="B312" t="n">
-        <v>100901.3108602124</v>
+        <v>100901.310860429</v>
       </c>
     </row>
     <row r="313">
@@ -2938,7 +2938,7 @@
         <v>1911</v>
       </c>
       <c r="B313" t="n">
-        <v>102518.5110511117</v>
+        <v>102518.5110513053</v>
       </c>
     </row>
     <row r="314">
@@ -2946,7 +2946,7 @@
         <v>1912</v>
       </c>
       <c r="B314" t="n">
-        <v>104162.4592961455</v>
+        <v>104162.4592963187</v>
       </c>
     </row>
     <row r="315">
@@ -2954,7 +2954,7 @@
         <v>1913</v>
       </c>
       <c r="B315" t="n">
-        <v>105833.3980713008</v>
+        <v>105833.3980714522</v>
       </c>
     </row>
     <row r="316">
@@ -2962,7 +2962,7 @@
         <v>1914</v>
       </c>
       <c r="B316" t="n">
-        <v>107531.55526512</v>
+        <v>107531.5552652485</v>
       </c>
     </row>
     <row r="317">
@@ -2970,7 +2970,7 @@
         <v>1915</v>
       </c>
       <c r="B317" t="n">
-        <v>109257.1430497207</v>
+        <v>109257.143049829</v>
       </c>
     </row>
     <row r="318">
@@ -2978,7 +2978,7 @@
         <v>1916</v>
       </c>
       <c r="B318" t="n">
-        <v>111010.356727047</v>
+        <v>111010.3567271311</v>
       </c>
     </row>
     <row r="319">
@@ -2986,7 +2986,7 @@
         <v>1917</v>
       </c>
       <c r="B319" t="n">
-        <v>112791.3735520751</v>
+        <v>112791.3735521338</v>
       </c>
     </row>
     <row r="320">
@@ -2994,7 +2994,7 @@
         <v>1918</v>
       </c>
       <c r="B320" t="n">
-        <v>114600.3515352117</v>
+        <v>114600.3515352476</v>
       </c>
     </row>
     <row r="321">
@@ -3002,7 +3002,7 @@
         <v>1919</v>
       </c>
       <c r="B321" t="n">
-        <v>116437.4282263228</v>
+        <v>116437.4282263347</v>
       </c>
     </row>
     <row r="322">
@@ -3010,7 +3010,7 @@
         <v>1920</v>
       </c>
       <c r="B322" t="n">
-        <v>118302.7194827578</v>
+        <v>118302.7194827431</v>
       </c>
     </row>
     <row r="323">
@@ -3018,7 +3018,7 @@
         <v>1921</v>
       </c>
       <c r="B323" t="n">
-        <v>120196.3182244761</v>
+        <v>120196.3182244335</v>
       </c>
     </row>
     <row r="324">
@@ -3026,7 +3026,7 @@
         <v>1922</v>
       </c>
       <c r="B324" t="n">
-        <v>122118.2931790851</v>
+        <v>122118.2931790186</v>
       </c>
     </row>
     <row r="325">
@@ -3034,7 +3034,7 @@
         <v>1923</v>
       </c>
       <c r="B325" t="n">
-        <v>124068.6876204429</v>
+        <v>124068.6876203486</v>
       </c>
     </row>
     <row r="326">
@@ -3042,7 +3042,7 @@
         <v>1924</v>
       </c>
       <c r="B326" t="n">
-        <v>126047.5181040914</v>
+        <v>126047.5181039668</v>
       </c>
     </row>
     <row r="327">
@@ -3050,7 +3050,7 @@
         <v>1925</v>
       </c>
       <c r="B327" t="n">
-        <v>128054.7732035716</v>
+        <v>128054.7732034205</v>
       </c>
     </row>
     <row r="328">
@@ -3058,7 +3058,7 @@
         <v>1926</v>
       </c>
       <c r="B328" t="n">
-        <v>130090.4122516834</v>
+        <v>130090.412251502</v>
       </c>
     </row>
     <row r="329">
@@ -3066,7 +3066,7 @@
         <v>1927</v>
       </c>
       <c r="B329" t="n">
-        <v>132154.36409096</v>
+        <v>132154.3640907482</v>
       </c>
     </row>
     <row r="330">
@@ -3074,7 +3074,7 @@
         <v>1928</v>
       </c>
       <c r="B330" t="n">
-        <v>134246.5258380295</v>
+        <v>134246.5258377835</v>
       </c>
     </row>
     <row r="331">
@@ -3082,7 +3082,7 @@
         <v>1929</v>
       </c>
       <c r="B331" t="n">
-        <v>136366.7616666898</v>
+        <v>136366.7616664135</v>
       </c>
     </row>
     <row r="332">
@@ -3090,7 +3090,7 @@
         <v>1930</v>
       </c>
       <c r="B332" t="n">
-        <v>138514.9016147816</v>
+        <v>138514.9016144763</v>
       </c>
     </row>
     <row r="333">
@@ -3098,7 +3098,7 @@
         <v>1931</v>
       </c>
       <c r="B333" t="n">
-        <v>140690.7404200932</v>
+        <v>140690.740419751</v>
       </c>
     </row>
     <row r="334">
@@ -3106,7 +3106,7 @@
         <v>1932</v>
       </c>
       <c r="B334" t="n">
-        <v>142894.0363909452</v>
+        <v>142894.0363905676</v>
       </c>
     </row>
     <row r="335">
@@ -3114,7 +3114,7 @@
         <v>1933</v>
       </c>
       <c r="B335" t="n">
-        <v>145124.5103170638</v>
+        <v>145124.5103166531</v>
       </c>
     </row>
     <row r="336">
@@ -3122,7 +3122,7 @@
         <v>1934</v>
       </c>
       <c r="B336" t="n">
-        <v>147381.844426711</v>
+        <v>147381.8444262636</v>
       </c>
     </row>
     <row r="337">
@@ -3130,7 +3130,7 @@
         <v>1935</v>
       </c>
       <c r="B337" t="n">
-        <v>149665.681396185</v>
+        <v>149665.6813957006</v>
       </c>
     </row>
     <row r="338">
@@ -3138,7 +3138,7 @@
         <v>1936</v>
       </c>
       <c r="B338" t="n">
-        <v>151975.6234178527</v>
+        <v>151975.6234173302</v>
       </c>
     </row>
     <row r="339">
@@ -3146,7 +3146,7 @@
         <v>1937</v>
       </c>
       <c r="B339" t="n">
-        <v>154311.2313330686</v>
+        <v>154311.2313325065</v>
       </c>
     </row>
     <row r="340">
@@ -3154,7 +3154,7 @@
         <v>1938</v>
       </c>
       <c r="B340" t="n">
-        <v>156672.0238366463</v>
+        <v>156672.0238360486</v>
       </c>
     </row>
     <row r="341">
@@ -3162,7 +3162,7 @@
         <v>1939</v>
       </c>
       <c r="B341" t="n">
-        <v>159057.4767591608</v>
+        <v>159057.4767585171</v>
       </c>
     </row>
     <row r="342">
@@ -3170,7 +3170,7 @@
         <v>1940</v>
       </c>
       <c r="B342" t="n">
-        <v>161467.0224338428</v>
+        <v>161467.022433162</v>
       </c>
     </row>
     <row r="343">
@@ -3178,7 +3178,7 @@
         <v>1941</v>
       </c>
       <c r="B343" t="n">
-        <v>163900.0491547308</v>
+        <v>163900.0491540026</v>
       </c>
     </row>
     <row r="344">
@@ -3186,7 +3186,7 @@
         <v>1942</v>
       </c>
       <c r="B344" t="n">
-        <v>166355.9007325691</v>
+        <v>166355.9007318026</v>
       </c>
     </row>
     <row r="345">
@@ -3194,7 +3194,7 @@
         <v>1943</v>
       </c>
       <c r="B345" t="n">
-        <v>168833.8761552153</v>
+        <v>168833.8761544013</v>
       </c>
     </row>
     <row r="346">
@@ -3202,7 +3202,7 @@
         <v>1944</v>
       </c>
       <c r="B346" t="n">
-        <v>171333.2293587682</v>
+        <v>171333.2293579105</v>
       </c>
     </row>
     <row r="347">
@@ -3210,7 +3210,7 @@
         <v>1945</v>
       </c>
       <c r="B347" t="n">
-        <v>173853.1691162469</v>
+        <v>173853.1691153431</v>
       </c>
     </row>
     <row r="348">
@@ -3218,7 +3218,7 @@
         <v>1946</v>
       </c>
       <c r="B348" t="n">
-        <v>176392.8590495294</v>
+        <v>176392.8590485819</v>
       </c>
     </row>
     <row r="349">
@@ -3226,7 +3226,7 @@
         <v>1947</v>
       </c>
       <c r="B349" t="n">
-        <v>178951.4177711401</v>
+        <v>178951.4177701385</v>
       </c>
     </row>
     <row r="350">
@@ -3234,7 +3234,7 @@
         <v>1948</v>
       </c>
       <c r="B350" t="n">
-        <v>181527.9191611617</v>
+        <v>181527.9191601124</v>
       </c>
     </row>
     <row r="351">
@@ -3242,7 +3242,7 @@
         <v>1949</v>
       </c>
       <c r="B351" t="n">
-        <v>184121.3927853182</v>
+        <v>184121.3927842239</v>
       </c>
     </row>
     <row r="352">
@@ -3250,7 +3250,7 @@
         <v>1950</v>
       </c>
       <c r="B352" t="n">
-        <v>186730.8244590356</v>
+        <v>186730.8244578872</v>
       </c>
     </row>
     <row r="353">
@@ -3258,7 +3258,7 @@
         <v>1951</v>
       </c>
       <c r="B353" t="n">
-        <v>189355.1569626348</v>
+        <v>189355.1569614347</v>
       </c>
     </row>
     <row r="354">
@@ -3266,7 +3266,7 @@
         <v>1952</v>
       </c>
       <c r="B354" t="n">
-        <v>191993.2909118975</v>
+        <v>191993.2909106471</v>
       </c>
     </row>
     <row r="355">
@@ -3274,7 +3274,7 @@
         <v>1953</v>
       </c>
       <c r="B355" t="n">
-        <v>194644.0857882107</v>
+        <v>194644.085786906</v>
       </c>
     </row>
     <row r="356">
@@ -3282,7 +3282,7 @@
         <v>1954</v>
       </c>
       <c r="B356" t="n">
-        <v>197306.3611316709</v>
+        <v>197306.3611303146</v>
       </c>
     </row>
     <row r="357">
@@ -3290,7 +3290,7 @@
         <v>1955</v>
       </c>
       <c r="B357" t="n">
-        <v>199978.8979002218</v>
+        <v>199978.8978988073</v>
       </c>
     </row>
     <row r="358">
@@ -3298,7 +3298,7 @@
         <v>1956</v>
       </c>
       <c r="B358" t="n">
-        <v>217816.5993111332</v>
+        <v>217816.5993095545</v>
       </c>
     </row>
     <row r="359">
@@ -3306,7 +3306,7 @@
         <v>1957</v>
       </c>
       <c r="B359" t="n">
-        <v>220706.9739227913</v>
+        <v>220706.9739211542</v>
       </c>
     </row>
     <row r="360">
@@ -3314,7 +3314,7 @@
         <v>1958</v>
       </c>
       <c r="B360" t="n">
-        <v>223604.2152717551</v>
+        <v>223604.2152700597</v>
       </c>
     </row>
     <row r="361">
@@ -3322,7 +3322,7 @@
         <v>1959</v>
       </c>
       <c r="B361" t="n">
-        <v>226506.8655326307</v>
+        <v>226506.8655308769</v>
       </c>
     </row>
     <row r="362">
@@ -3330,7 +3330,7 @@
         <v>1960</v>
       </c>
       <c r="B362" t="n">
-        <v>229413.4354609017</v>
+        <v>229413.4354590811</v>
       </c>
     </row>
     <row r="363">
@@ -3338,7 +3338,7 @@
         <v>1961</v>
       </c>
       <c r="B363" t="n">
-        <v>232322.4069550165</v>
+        <v>232322.4069531347</v>
       </c>
     </row>
     <row r="364">
@@ -3346,7 +3346,7 @@
         <v>1962</v>
       </c>
       <c r="B364" t="n">
-        <v>235232.2358005846</v>
+        <v>235232.2357986443</v>
       </c>
     </row>
     <row r="365">
@@ -3354,7 +3354,7 @@
         <v>1963</v>
       </c>
       <c r="B365" t="n">
-        <v>238141.3545935237</v>
+        <v>238141.3545915138</v>
       </c>
     </row>
     <row r="366">
@@ -3362,7 +3362,7 @@
         <v>1964</v>
       </c>
       <c r="B366" t="n">
-        <v>241048.1758388956</v>
+        <v>241048.1758368273</v>
       </c>
     </row>
     <row r="367">
@@ -3370,7 +3370,7 @@
         <v>1965</v>
       </c>
       <c r="B367" t="n">
-        <v>243951.0952212831</v>
+        <v>243951.0952191563</v>
       </c>
     </row>
     <row r="368">
@@ -3378,7 +3378,7 @@
         <v>1966</v>
       </c>
       <c r="B368" t="n">
-        <v>246848.4950409575</v>
+        <v>246848.4950387666</v>
       </c>
     </row>
     <row r="369">
@@ -3386,7 +3386,7 @@
         <v>1967</v>
       </c>
       <c r="B369" t="n">
-        <v>249738.7478103951</v>
+        <v>249738.7478081458</v>
       </c>
     </row>
     <row r="370">
@@ -3394,7 +3394,7 @@
         <v>1968</v>
       </c>
       <c r="B370" t="n">
-        <v>252620.2200035911</v>
+        <v>252620.2200012721</v>
       </c>
     </row>
     <row r="371">
@@ -3402,7 +3402,7 @@
         <v>1969</v>
       </c>
       <c r="B371" t="n">
-        <v>255491.2759507617</v>
+        <v>255491.2759483842</v>
       </c>
     </row>
     <row r="372">
@@ -3410,7 +3410,7 @@
         <v>1970</v>
       </c>
       <c r="B372" t="n">
-        <v>258350.2818697478</v>
+        <v>258350.2818673174</v>
       </c>
     </row>
     <row r="373">
@@ -3418,7 +3418,7 @@
         <v>1971</v>
       </c>
       <c r="B373" t="n">
-        <v>254283.9628051224</v>
+        <v>254283.9628026885</v>
       </c>
     </row>
     <row r="374">
@@ -3426,7 +3426,7 @@
         <v>1972</v>
       </c>
       <c r="B374" t="n">
-        <v>257039.1086512413</v>
+        <v>257039.1086487586</v>
       </c>
     </row>
     <row r="375">
@@ -3434,7 +3434,7 @@
         <v>1973</v>
       </c>
       <c r="B375" t="n">
-        <v>259777.8037519292</v>
+        <v>259777.8037493922</v>
       </c>
     </row>
     <row r="376">
@@ -3442,7 +3442,7 @@
         <v>1974</v>
       </c>
       <c r="B376" t="n">
-        <v>262498.5064773588</v>
+        <v>262498.5064747595</v>
       </c>
     </row>
     <row r="377">
@@ -3450,7 +3450,7 @@
         <v>1975</v>
       </c>
       <c r="B377" t="n">
-        <v>265199.6983062237</v>
+        <v>265199.6983035783</v>
       </c>
     </row>
     <row r="378">
@@ -3458,7 +3458,7 @@
         <v>1976</v>
       </c>
       <c r="B378" t="n">
-        <v>267879.8883301202</v>
+        <v>267879.8883274152</v>
       </c>
     </row>
     <row r="379">
@@ -3466,7 +3466,7 @@
         <v>1977</v>
       </c>
       <c r="B379" t="n">
-        <v>270537.6178119734</v>
+        <v>270537.6178092304</v>
       </c>
     </row>
     <row r="380">
@@ -3474,7 +3474,7 @@
         <v>1978</v>
       </c>
       <c r="B380" t="n">
-        <v>273171.4647848681</v>
+        <v>273171.4647820789</v>
       </c>
     </row>
     <row r="381">
@@ -3482,7 +3482,7 @@
         <v>1979</v>
       </c>
       <c r="B381" t="n">
-        <v>275780.048677278</v>
+        <v>275780.0486744373</v>
       </c>
     </row>
     <row r="382">
@@ -3490,7 +3490,7 @@
         <v>1980</v>
       </c>
       <c r="B382" t="n">
-        <v>278362.0349501816</v>
+        <v>278362.0349473056</v>
       </c>
     </row>
     <row r="383">
@@ -3498,7 +3498,7 @@
         <v>1981</v>
       </c>
       <c r="B383" t="n">
-        <v>215236.5443044131</v>
+        <v>215236.5443021783</v>
       </c>
     </row>
     <row r="384">
@@ -3506,7 +3506,7 @@
         <v>1982</v>
       </c>
       <c r="B384" t="n">
-        <v>217171.1826432301</v>
+        <v>217171.1826409725</v>
       </c>
     </row>
     <row r="385">
@@ -3514,7 +3514,7 @@
         <v>1983</v>
       </c>
       <c r="B385" t="n">
-        <v>219082.6215159229</v>
+        <v>219082.6215136362</v>
       </c>
     </row>
     <row r="386">
@@ -3522,7 +3522,7 @@
         <v>1984</v>
       </c>
       <c r="B386" t="n">
-        <v>220970.0147998908</v>
+        <v>220970.0147975875</v>
       </c>
     </row>
     <row r="387">
@@ -3530,7 +3530,7 @@
         <v>1985</v>
       </c>
       <c r="B387" t="n">
-        <v>222832.5691449723</v>
+        <v>222832.5691426523</v>
       </c>
     </row>
     <row r="388">
@@ -3538,7 +3538,7 @@
         <v>1986</v>
       </c>
       <c r="B388" t="n">
-        <v>224669.5473402231</v>
+        <v>224669.5473378844</v>
       </c>
     </row>
     <row r="389">
@@ -3546,7 +3546,7 @@
         <v>1987</v>
       </c>
       <c r="B389" t="n">
-        <v>226480.2716090042</v>
+        <v>226480.2716066613</v>
       </c>
     </row>
     <row r="390">
@@ -3554,7 +3554,7 @@
         <v>1988</v>
       </c>
       <c r="B390" t="n">
-        <v>228264.1268209793</v>
+        <v>228264.1268186281</v>
       </c>
     </row>
     <row r="391">
@@ -3562,7 +3562,7 @@
         <v>1989</v>
       </c>
       <c r="B391" t="n">
-        <v>230020.5636096019</v>
+        <v>230020.5636072569</v>
       </c>
     </row>
     <row r="392">
@@ -3570,7 +3570,7 @@
         <v>1990</v>
       </c>
       <c r="B392" t="n">
-        <v>231749.1013841411</v>
+        <v>231749.1013817939</v>
       </c>
     </row>
     <row r="393">
@@ -3578,7 +3578,7 @@
         <v>1991</v>
       </c>
       <c r="B393" t="n">
-        <v>343367.4969921544</v>
+        <v>343367.4969887233</v>
       </c>
     </row>
     <row r="394">
@@ -3586,7 +3586,7 @@
         <v>1992</v>
       </c>
       <c r="B394" t="n">
-        <v>345826.1409646957</v>
+        <v>345826.1409612798</v>
       </c>
     </row>
     <row r="395">
@@ -3594,7 +3594,7 @@
         <v>1993</v>
       </c>
       <c r="B395" t="n">
-        <v>348242.2778140905</v>
+        <v>348242.2778107051</v>
       </c>
     </row>
     <row r="396">
@@ -3602,7 +3602,7 @@
         <v>1994</v>
       </c>
       <c r="B396" t="n">
-        <v>350615.645944871</v>
+        <v>350615.6459415283</v>
       </c>
     </row>
     <row r="397">
@@ -3610,7 +3610,7 @@
         <v>1995</v>
       </c>
       <c r="B397" t="n">
-        <v>352946.1041959572</v>
+        <v>352946.1041926633</v>
       </c>
     </row>
     <row r="398">
@@ -3618,7 +3618,7 @@
         <v>1996</v>
       </c>
       <c r="B398" t="n">
-        <v>355233.6350174868</v>
+        <v>355233.6350142568</v>
       </c>
     </row>
     <row r="399">
@@ -3626,7 +3626,7 @@
         <v>1997</v>
       </c>
       <c r="B399" t="n">
-        <v>357478.3473894878</v>
+        <v>357478.3473863279</v>
       </c>
     </row>
     <row r="400">
@@ -3634,7 +3634,7 @@
         <v>1998</v>
       </c>
       <c r="B400" t="n">
-        <v>359680.4794688068</v>
+        <v>359680.4794657293</v>
       </c>
     </row>
     <row r="401">
@@ -3642,7 +3642,7 @@
         <v>1999</v>
       </c>
       <c r="B401" t="n">
-        <v>361840.4009527031</v>
+        <v>361840.4009497202</v>
       </c>
     </row>
     <row r="402">
@@ -3650,7 +3650,7 @@
         <v>2000</v>
       </c>
       <c r="B402" t="n">
-        <v>363958.6151459903</v>
+        <v>363958.6151431201</v>
       </c>
     </row>
     <row r="403">
@@ -3658,7 +3658,7 @@
         <v>2001</v>
       </c>
       <c r="B403" t="n">
-        <v>983043.8436066696</v>
+        <v>983043.8435992725</v>
       </c>
     </row>
     <row r="404">
@@ -3666,7 +3666,7 @@
         <v>2002</v>
       </c>
       <c r="B404" t="n">
-        <v>988514.1158130482</v>
+        <v>988514.1158060362</v>
       </c>
     </row>
     <row r="405">
@@ -3674,7 +3674,7 @@
         <v>2003</v>
       </c>
       <c r="B405" t="n">
-        <v>993878.6278342606</v>
+        <v>993878.6278276336</v>
       </c>
     </row>
     <row r="406">
@@ -3682,7 +3682,7 @@
         <v>2004</v>
       </c>
       <c r="B406" t="n">
-        <v>999140.2052091751</v>
+        <v>999140.2052029987</v>
       </c>
     </row>
     <row r="407">
@@ -3690,7 +3690,7 @@
         <v>2005</v>
       </c>
       <c r="B407" t="n">
-        <v>1004302.047068411</v>
+        <v>1004302.047062751</v>
       </c>
     </row>
     <row r="408">
@@ -3698,7 +3698,7 @@
         <v>2006</v>
       </c>
       <c r="B408" t="n">
-        <v>1009367.726283663</v>
+        <v>1009367.726278511</v>
       </c>
     </row>
     <row r="409">
@@ -3706,7 +3706,7 @@
         <v>2007</v>
       </c>
       <c r="B409" t="n">
-        <v>1014341.188617754</v>
+        <v>1014341.188613184</v>
       </c>
     </row>
     <row r="410">
@@ -3714,7 +3714,7 @@
         <v>2008</v>
       </c>
       <c r="B410" t="n">
-        <v>1019226.750843105</v>
+        <v>1019226.750839165</v>
       </c>
     </row>
     <row r="411">
@@ -3722,7 +3722,7 @@
         <v>2009</v>
       </c>
       <c r="B411" t="n">
-        <v>1024029.097804603</v>
+        <v>1024029.097801327</v>
       </c>
     </row>
     <row r="412">
@@ -3730,7 +3730,7 @@
         <v>2010</v>
       </c>
       <c r="B412" t="n">
-        <v>1028753.278393618</v>
+        <v>1028753.278391095</v>
       </c>
     </row>
     <row r="413">
@@ -3738,7 +3738,7 @@
         <v>2011</v>
       </c>
       <c r="B413" t="n">
-        <v>1115583.896842943</v>
+        <v>1115583.896841086</v>
       </c>
     </row>
     <row r="414">
@@ -3746,7 +3746,7 @@
         <v>2012</v>
       </c>
       <c r="B414" t="n">
-        <v>1120532.886744793</v>
+        <v>1120532.88674382</v>
       </c>
     </row>
     <row r="415">
@@ -3754,7 +3754,7 @@
         <v>2013</v>
       </c>
       <c r="B415" t="n">
-        <v>1125416.141705901</v>
+        <v>1125416.141705866</v>
       </c>
     </row>
     <row r="416">
@@ -3762,7 +3762,7 @@
         <v>2014</v>
       </c>
       <c r="B416" t="n">
-        <v>1130240.616060636</v>
+        <v>1130240.616061627</v>
       </c>
     </row>
     <row r="417">
@@ -3770,7 +3770,7 @@
         <v>2015</v>
       </c>
       <c r="B417" t="n">
-        <v>1135013.616674762</v>
+        <v>1135013.616676885</v>
       </c>
     </row>
     <row r="418">
@@ -3778,7 +3778,7 @@
         <v>2016</v>
       </c>
       <c r="B418" t="n">
-        <v>1139742.790863914</v>
+        <v>1139742.790867169</v>
       </c>
     </row>
     <row r="419">
@@ -3786,7 +3786,7 @@
         <v>2017</v>
       </c>
       <c r="B419" t="n">
-        <v>1144436.112898908</v>
+        <v>1144436.112903384</v>
       </c>
     </row>
     <row r="420">
@@ -3794,7 +3794,7 @@
         <v>2018</v>
       </c>
       <c r="B420" t="n">
-        <v>1149101.869059497</v>
+        <v>1149101.869065282</v>
       </c>
     </row>
     <row r="421">
@@ -3802,7 +3802,7 @@
         <v>2019</v>
       </c>
       <c r="B421" t="n">
-        <v>1153748.641199037</v>
+        <v>1153748.641206148</v>
       </c>
     </row>
     <row r="422">
@@ -3810,7 +3810,7 @@
         <v>2020</v>
       </c>
       <c r="B422" t="n">
-        <v>1158385.28878004</v>
+        <v>1158385.288788548</v>
       </c>
     </row>
     <row r="423">
@@ -3818,7 +3818,7 @@
         <v>2021</v>
       </c>
       <c r="B423" t="n">
-        <v>1163020.929344759</v>
+        <v>1163020.929354771</v>
       </c>
     </row>
     <row r="424">
@@ -3826,7 +3826,7 @@
         <v>2022</v>
       </c>
       <c r="B424" t="n">
-        <v>1167664.917379638</v>
+        <v>1167664.917391207</v>
       </c>
     </row>
     <row r="425">
@@ -3834,7 +3834,7 @@
         <v>2023</v>
       </c>
       <c r="B425" t="n">
-        <v>1172326.821540681</v>
+        <v>1172326.82155386</v>
       </c>
     </row>
     <row r="426">
@@ -3842,7 +3842,7 @@
         <v>2024</v>
       </c>
       <c r="B426" t="n">
-        <v>1177016.400200688</v>
+        <v>1177016.400215529</v>
       </c>
     </row>
     <row r="427">
@@ -3850,7 +3850,7 @@
         <v>2025</v>
       </c>
       <c r="B427" t="n">
-        <v>1181743.575288674</v>
+        <v>1181743.575305284</v>
       </c>
     </row>
     <row r="428">
@@ -3858,7 +3858,7 @@
         <v>2026</v>
       </c>
       <c r="B428" t="n">
-        <v>1186518.404391232</v>
+        <v>1186518.404409646</v>
       </c>
     </row>
     <row r="429">
@@ -3866,7 +3866,7 @@
         <v>2027</v>
       </c>
       <c r="B429" t="n">
-        <v>1191351.05108934</v>
+        <v>1191351.051109594</v>
       </c>
     </row>
     <row r="430">
@@ -3874,7 +3874,7 @@
         <v>2028</v>
       </c>
       <c r="B430" t="n">
-        <v>1196251.753512539</v>
+        <v>1196251.753534775</v>
       </c>
     </row>
     <row r="431">
@@ -3882,7 +3882,7 @@
         <v>2029</v>
       </c>
       <c r="B431" t="n">
-        <v>1201230.791095426</v>
+        <v>1201230.791119607</v>
       </c>
     </row>
     <row r="432">
@@ -3890,7 +3890,7 @@
         <v>2030</v>
       </c>
       <c r="B432" t="n">
-        <v>1206298.449529908</v>
+        <v>1206298.449556088</v>
       </c>
     </row>
     <row r="433">
@@ -3898,7 +3898,7 @@
         <v>2031</v>
       </c>
       <c r="B433" t="n">
-        <v>1211464.983917283</v>
+        <v>1211464.983945585</v>
       </c>
     </row>
     <row r="434">
@@ -3906,7 +3906,7 @@
         <v>2032</v>
       </c>
       <c r="B434" t="n">
-        <v>1216740.580130534</v>
+        <v>1216740.580160995</v>
       </c>
     </row>
     <row r="435">
@@ -3914,7 +3914,7 @@
         <v>2033</v>
       </c>
       <c r="B435" t="n">
-        <v>1222135.314413717</v>
+        <v>1222135.314446336</v>
       </c>
     </row>
     <row r="436">
@@ -3922,7 +3922,7 @@
         <v>2034</v>
       </c>
       <c r="B436" t="n">
-        <v>1227659.111252251</v>
+        <v>1227659.111287027</v>
       </c>
     </row>
     <row r="437">
@@ -3930,7 +3930,7 @@
         <v>2035</v>
       </c>
       <c r="B437" t="n">
-        <v>1233321.699569666</v>
+        <v>1233321.699606741</v>
       </c>
     </row>
     <row r="438">
@@ -3938,7 +3938,7 @@
         <v>2036</v>
       </c>
       <c r="B438" t="n">
-        <v>1239132.567314676</v>
+        <v>1239132.567353963</v>
       </c>
     </row>
     <row r="439">
@@ -3946,7 +3946,7 @@
         <v>2037</v>
       </c>
       <c r="B439" t="n">
-        <v>1245100.914527719</v>
+        <v>1245100.914569288</v>
       </c>
     </row>
     <row r="440">
@@ -3954,7 +3954,7 @@
         <v>2038</v>
       </c>
       <c r="B440" t="n">
-        <v>1251235.60498753</v>
+        <v>1251235.605031416</v>
       </c>
     </row>
     <row r="441">
@@ -3962,7 +3962,7 @@
         <v>2039</v>
       </c>
       <c r="B441" t="n">
-        <v>1257545.116565706</v>
+        <v>1257545.116611891</v>
       </c>
     </row>
     <row r="442">
@@ -3970,7 +3970,7 @@
         <v>2040</v>
       </c>
       <c r="B442" t="n">
-        <v>1264037.490434306</v>
+        <v>1264037.490482774</v>
       </c>
     </row>
     <row r="443">
@@ -3978,7 +3978,7 @@
         <v>2041</v>
       </c>
       <c r="B443" t="n">
-        <v>1270720.279295618</v>
+        <v>1270720.27934635</v>
       </c>
     </row>
     <row r="444">
@@ -3986,7 +3986,7 @@
         <v>2042</v>
       </c>
       <c r="B444" t="n">
-        <v>1277600.494829536</v>
+        <v>1277600.494882549</v>
       </c>
     </row>
     <row r="445">
@@ -3994,7 +3994,7 @@
         <v>2043</v>
       </c>
       <c r="B445" t="n">
-        <v>1284684.554576099</v>
+        <v>1284684.554631306</v>
       </c>
     </row>
     <row r="446">
@@ -4002,7 +4002,7 @@
         <v>2044</v>
       </c>
       <c r="B446" t="n">
-        <v>1291978.228498197</v>
+        <v>1291978.228555633</v>
       </c>
     </row>
     <row r="447">
@@ -4010,7 +4010,7 @@
         <v>2045</v>
       </c>
       <c r="B447" t="n">
-        <v>1299486.585494871</v>
+        <v>1299486.585554376</v>
       </c>
     </row>
     <row r="448">
@@ -4018,7 +4018,7 @@
         <v>2046</v>
       </c>
       <c r="B448" t="n">
-        <v>1307213.94016231</v>
+        <v>1307213.940223921</v>
       </c>
     </row>
     <row r="449">
@@ -4026,7 +4026,7 @@
         <v>2047</v>
       </c>
       <c r="B449" t="n">
-        <v>1315163.800127917</v>
+        <v>1315163.800191544</v>
       </c>
     </row>
     <row r="450">
@@ -4034,7 +4034,7 @@
         <v>2048</v>
       </c>
       <c r="B450" t="n">
-        <v>1323338.814301805</v>
+        <v>1323338.814367307</v>
       </c>
     </row>
     <row r="451">
@@ -4042,7 +4042,7 @@
         <v>2049</v>
       </c>
       <c r="B451" t="n">
-        <v>1331740.722425331</v>
+        <v>1331740.722492638</v>
       </c>
     </row>
     <row r="452">
@@ -4050,7 +4050,7 @@
         <v>2050</v>
       </c>
       <c r="B452" t="n">
-        <v>1340370.306310536</v>
+        <v>1340370.306379611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>